<commit_message>
serienbrief merge: code adapted to kibon
</commit_message>
<xml_diff>
--- a/ebegu-server/src/main/resources/reporting/Massenversand.xlsx
+++ b/ebegu-server/src/main/resources/reporting/Massenversand.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Client\G$\hefr\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Client\A$\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C886365A-A591-4E5E-8D6F-C29896856D2E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C47692AD-F7B9-42B6-AAAB-7DFFAEA846DF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="435" windowWidth="33600" windowHeight="20565" tabRatio="606" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="975" yWindow="795" windowWidth="33600" windowHeight="20565" tabRatio="606" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="6" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="70">
   <si>
     <t>Parameter</t>
   </si>
@@ -234,6 +234,12 @@
   </si>
   <si>
     <t>Kontaktdaten für Serienbriefe</t>
+  </si>
+  <si>
+    <t>{kindInstitutionTagesfamilie}</t>
+  </si>
+  <si>
+    <t>Tagesfamilie</t>
   </si>
 </sst>
 </file>
@@ -435,8 +441,13 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -457,13 +468,8 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+      <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -873,10 +879,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:DV16"/>
+  <dimension ref="A1:DT16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K33" sqref="K33"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="T23" sqref="T23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -894,79 +900,78 @@
     <col min="12" max="12" width="11.140625" customWidth="1"/>
     <col min="13" max="13" width="10.140625" customWidth="1"/>
     <col min="14" max="14" width="18.140625"/>
-    <col min="18" max="18" width="22.85546875" customWidth="1"/>
-    <col min="19" max="19" width="23" customWidth="1"/>
-    <col min="20" max="20" width="25.85546875" customWidth="1"/>
-    <col min="21" max="21" width="17.42578125" customWidth="1"/>
-    <col min="22" max="22" width="24.28515625" customWidth="1"/>
-    <col min="23" max="23" width="11.140625" customWidth="1"/>
-    <col min="24" max="24" width="10.140625" customWidth="1"/>
-    <col min="29" max="29" width="22.85546875" customWidth="1"/>
-    <col min="30" max="30" width="23" customWidth="1"/>
-    <col min="31" max="31" width="25.85546875" customWidth="1"/>
-    <col min="32" max="32" width="17.42578125" customWidth="1"/>
-    <col min="33" max="33" width="24.28515625" customWidth="1"/>
-    <col min="34" max="34" width="11.140625" customWidth="1"/>
-    <col min="35" max="35" width="10.140625" customWidth="1"/>
-    <col min="40" max="40" width="22.85546875" customWidth="1"/>
-    <col min="41" max="41" width="23" customWidth="1"/>
-    <col min="42" max="42" width="25.85546875" customWidth="1"/>
-    <col min="43" max="43" width="17.42578125" customWidth="1"/>
-    <col min="44" max="44" width="24.28515625" customWidth="1"/>
-    <col min="45" max="45" width="11.140625" customWidth="1"/>
-    <col min="46" max="46" width="10.140625" customWidth="1"/>
-    <col min="51" max="51" width="22.85546875" customWidth="1"/>
-    <col min="52" max="52" width="23" customWidth="1"/>
-    <col min="53" max="53" width="25.85546875" customWidth="1"/>
-    <col min="54" max="54" width="17.42578125" customWidth="1"/>
-    <col min="55" max="55" width="24.28515625" customWidth="1"/>
-    <col min="56" max="56" width="11.140625" customWidth="1"/>
-    <col min="57" max="57" width="10.140625" customWidth="1"/>
-    <col min="62" max="62" width="22.85546875" customWidth="1"/>
-    <col min="63" max="63" width="23" customWidth="1"/>
-    <col min="64" max="64" width="25.85546875" customWidth="1"/>
-    <col min="65" max="65" width="17.42578125" customWidth="1"/>
-    <col min="66" max="66" width="24.28515625" customWidth="1"/>
-    <col min="67" max="67" width="11.140625" customWidth="1"/>
-    <col min="68" max="68" width="10.140625" customWidth="1"/>
-    <col min="73" max="73" width="22.85546875" customWidth="1"/>
-    <col min="74" max="74" width="23" customWidth="1"/>
-    <col min="75" max="75" width="25.85546875" customWidth="1"/>
-    <col min="76" max="76" width="17.42578125" customWidth="1"/>
-    <col min="77" max="77" width="24.28515625" customWidth="1"/>
-    <col min="78" max="78" width="11.140625" customWidth="1"/>
-    <col min="79" max="79" width="10.140625" customWidth="1"/>
-    <col min="84" max="84" width="22.85546875" customWidth="1"/>
-    <col min="85" max="85" width="23" customWidth="1"/>
-    <col min="86" max="86" width="25.85546875" customWidth="1"/>
-    <col min="87" max="87" width="17.42578125" customWidth="1"/>
-    <col min="88" max="88" width="24.28515625" customWidth="1"/>
-    <col min="89" max="89" width="11.140625" customWidth="1"/>
-    <col min="90" max="90" width="10.140625" customWidth="1"/>
-    <col min="95" max="95" width="22.85546875" customWidth="1"/>
-    <col min="96" max="96" width="23" customWidth="1"/>
-    <col min="97" max="97" width="25.85546875" customWidth="1"/>
-    <col min="98" max="98" width="17.42578125" customWidth="1"/>
-    <col min="99" max="99" width="24.28515625" customWidth="1"/>
-    <col min="100" max="100" width="11.140625" customWidth="1"/>
-    <col min="101" max="101" width="10.140625" customWidth="1"/>
-    <col min="106" max="106" width="22.85546875" customWidth="1"/>
-    <col min="107" max="107" width="23" customWidth="1"/>
-    <col min="108" max="108" width="25.85546875" customWidth="1"/>
-    <col min="109" max="109" width="17.42578125" customWidth="1"/>
-    <col min="110" max="110" width="24.28515625" customWidth="1"/>
-    <col min="111" max="111" width="11.140625" customWidth="1"/>
-    <col min="112" max="112" width="10.140625" customWidth="1"/>
-    <col min="117" max="117" width="22.85546875" customWidth="1"/>
-    <col min="118" max="118" width="23" customWidth="1"/>
-    <col min="119" max="119" width="25.85546875" customWidth="1"/>
-    <col min="120" max="120" width="17.42578125" customWidth="1"/>
-    <col min="121" max="123" width="24.28515625" customWidth="1"/>
-    <col min="124" max="124" width="15.7109375" customWidth="1"/>
-    <col min="125" max="1036" width="10.42578125"/>
+    <col min="17" max="17" width="19" customWidth="1"/>
+    <col min="18" max="18" width="25.85546875" customWidth="1"/>
+    <col min="19" max="19" width="17.42578125" customWidth="1"/>
+    <col min="20" max="20" width="24.28515625" customWidth="1"/>
+    <col min="21" max="21" width="11.140625" customWidth="1"/>
+    <col min="22" max="22" width="10.140625" customWidth="1"/>
+    <col min="27" max="27" width="22.85546875" customWidth="1"/>
+    <col min="28" max="28" width="23" customWidth="1"/>
+    <col min="29" max="29" width="25.85546875" customWidth="1"/>
+    <col min="30" max="30" width="17.42578125" customWidth="1"/>
+    <col min="31" max="31" width="24.28515625" customWidth="1"/>
+    <col min="32" max="32" width="11.140625" customWidth="1"/>
+    <col min="33" max="33" width="10.140625" customWidth="1"/>
+    <col min="38" max="38" width="22.85546875" customWidth="1"/>
+    <col min="39" max="39" width="23" customWidth="1"/>
+    <col min="40" max="40" width="25.85546875" customWidth="1"/>
+    <col min="41" max="41" width="17.42578125" customWidth="1"/>
+    <col min="42" max="42" width="24.28515625" customWidth="1"/>
+    <col min="43" max="43" width="11.140625" customWidth="1"/>
+    <col min="44" max="44" width="10.140625" customWidth="1"/>
+    <col min="49" max="49" width="22.85546875" customWidth="1"/>
+    <col min="50" max="50" width="23" customWidth="1"/>
+    <col min="51" max="51" width="25.85546875" customWidth="1"/>
+    <col min="52" max="52" width="17.42578125" customWidth="1"/>
+    <col min="53" max="53" width="24.28515625" customWidth="1"/>
+    <col min="54" max="54" width="11.140625" customWidth="1"/>
+    <col min="55" max="55" width="10.140625" customWidth="1"/>
+    <col min="60" max="60" width="22.85546875" customWidth="1"/>
+    <col min="61" max="61" width="23" customWidth="1"/>
+    <col min="62" max="62" width="25.85546875" customWidth="1"/>
+    <col min="63" max="63" width="17.42578125" customWidth="1"/>
+    <col min="64" max="64" width="24.28515625" customWidth="1"/>
+    <col min="65" max="65" width="11.140625" customWidth="1"/>
+    <col min="66" max="66" width="10.140625" customWidth="1"/>
+    <col min="71" max="71" width="22.85546875" customWidth="1"/>
+    <col min="72" max="72" width="23" customWidth="1"/>
+    <col min="73" max="73" width="25.85546875" customWidth="1"/>
+    <col min="74" max="74" width="17.42578125" customWidth="1"/>
+    <col min="75" max="75" width="24.28515625" customWidth="1"/>
+    <col min="76" max="76" width="11.140625" customWidth="1"/>
+    <col min="77" max="77" width="10.140625" customWidth="1"/>
+    <col min="82" max="82" width="22.85546875" customWidth="1"/>
+    <col min="83" max="83" width="23" customWidth="1"/>
+    <col min="84" max="84" width="25.85546875" customWidth="1"/>
+    <col min="85" max="85" width="17.42578125" customWidth="1"/>
+    <col min="86" max="86" width="24.28515625" customWidth="1"/>
+    <col min="87" max="87" width="11.140625" customWidth="1"/>
+    <col min="88" max="88" width="10.140625" customWidth="1"/>
+    <col min="93" max="93" width="22.85546875" customWidth="1"/>
+    <col min="94" max="94" width="23" customWidth="1"/>
+    <col min="95" max="95" width="25.85546875" customWidth="1"/>
+    <col min="96" max="96" width="17.42578125" customWidth="1"/>
+    <col min="97" max="97" width="24.28515625" customWidth="1"/>
+    <col min="98" max="98" width="11.140625" customWidth="1"/>
+    <col min="99" max="99" width="10.140625" customWidth="1"/>
+    <col min="104" max="104" width="22.85546875" customWidth="1"/>
+    <col min="105" max="105" width="23" customWidth="1"/>
+    <col min="106" max="106" width="25.85546875" customWidth="1"/>
+    <col min="107" max="107" width="17.42578125" customWidth="1"/>
+    <col min="108" max="108" width="24.28515625" customWidth="1"/>
+    <col min="109" max="109" width="11.140625" customWidth="1"/>
+    <col min="110" max="110" width="10.140625" customWidth="1"/>
+    <col min="115" max="115" width="22.85546875" customWidth="1"/>
+    <col min="116" max="116" width="23" customWidth="1"/>
+    <col min="117" max="117" width="25.85546875" customWidth="1"/>
+    <col min="118" max="118" width="17.42578125" customWidth="1"/>
+    <col min="119" max="121" width="24.28515625" customWidth="1"/>
+    <col min="122" max="122" width="15.7109375" customWidth="1"/>
+    <col min="123" max="1034" width="10.42578125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:126" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:124" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>67</v>
       </c>
@@ -977,10 +982,10 @@
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
     </row>
-    <row r="2" spans="1:126" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:124" x14ac:dyDescent="0.25">
       <c r="C2"/>
     </row>
-    <row r="3" spans="1:126" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:124" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>0</v>
       </c>
@@ -991,7 +996,7 @@
       <c r="F3" s="4"/>
       <c r="G3" s="4"/>
     </row>
-    <row r="4" spans="1:126" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:124" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -1000,7 +1005,7 @@
       </c>
       <c r="C4"/>
     </row>
-    <row r="5" spans="1:126" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:124" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -1009,7 +1014,7 @@
       </c>
       <c r="C5"/>
     </row>
-    <row r="6" spans="1:126" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:124" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>1</v>
       </c>
@@ -1018,7 +1023,7 @@
       </c>
       <c r="C6"/>
     </row>
-    <row r="7" spans="1:126" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:124" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>20</v>
       </c>
@@ -1027,7 +1032,7 @@
       </c>
       <c r="C7"/>
     </row>
-    <row r="8" spans="1:126" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:124" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>21</v>
       </c>
@@ -1036,7 +1041,7 @@
       </c>
       <c r="C8"/>
     </row>
-    <row r="9" spans="1:126" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:124" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>22</v>
       </c>
@@ -1045,7 +1050,7 @@
       </c>
       <c r="C9"/>
     </row>
-    <row r="10" spans="1:126" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:124" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>23</v>
       </c>
@@ -1054,19 +1059,19 @@
       </c>
       <c r="C10"/>
     </row>
-    <row r="11" spans="1:126" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:124" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="27" t="s">
+      <c r="B11" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="C11" s="28"/>
+      <c r="C11" s="20"/>
       <c r="D11" s="8"/>
       <c r="E11" s="8"/>
       <c r="F11" s="8"/>
     </row>
-    <row r="12" spans="1:126" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:124" x14ac:dyDescent="0.25">
       <c r="C12"/>
       <c r="L12" t="s">
         <v>55</v>
@@ -1392,684 +1397,668 @@
       <c r="DO12" t="s">
         <v>55</v>
       </c>
-      <c r="DP12" t="s">
-        <v>55</v>
-      </c>
-      <c r="DQ12" t="s">
-        <v>55</v>
-      </c>
     </row>
-    <row r="13" spans="1:126" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="25" t="s">
+    <row r="13" spans="1:124" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="B13" s="25" t="s">
+      <c r="B13" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="C13" s="18" t="s">
+      <c r="C13" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="D13" s="18"/>
-      <c r="E13" s="18"/>
-      <c r="F13" s="18"/>
-      <c r="G13" s="18" t="s">
+      <c r="D13" s="28"/>
+      <c r="E13" s="28"/>
+      <c r="F13" s="28"/>
+      <c r="G13" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="H13" s="18"/>
-      <c r="I13" s="18"/>
-      <c r="J13" s="18"/>
-      <c r="K13" s="25" t="s">
+      <c r="H13" s="28"/>
+      <c r="I13" s="28"/>
+      <c r="J13" s="28"/>
+      <c r="K13" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="L13" s="18" t="s">
+      <c r="L13" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="M13" s="18"/>
-      <c r="N13" s="18"/>
-      <c r="O13" s="18"/>
-      <c r="P13" s="18"/>
-      <c r="Q13" s="18"/>
-      <c r="R13" s="18"/>
-      <c r="S13" s="18"/>
-      <c r="T13" s="18"/>
-      <c r="U13" s="18"/>
-      <c r="V13" s="18"/>
-      <c r="W13" s="18" t="s">
+      <c r="M13" s="28"/>
+      <c r="N13" s="28"/>
+      <c r="O13" s="28"/>
+      <c r="P13" s="28"/>
+      <c r="Q13" s="28"/>
+      <c r="R13" s="28"/>
+      <c r="S13" s="28"/>
+      <c r="T13" s="28"/>
+      <c r="U13" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="X13" s="18"/>
-      <c r="Y13" s="18"/>
-      <c r="Z13" s="18"/>
-      <c r="AA13" s="18"/>
-      <c r="AB13" s="18"/>
-      <c r="AC13" s="18"/>
-      <c r="AD13" s="18"/>
-      <c r="AE13" s="18"/>
-      <c r="AF13" s="18"/>
-      <c r="AG13" s="18"/>
-      <c r="AH13" s="18" t="s">
+      <c r="V13" s="28"/>
+      <c r="W13" s="28"/>
+      <c r="X13" s="28"/>
+      <c r="Y13" s="28"/>
+      <c r="Z13" s="28"/>
+      <c r="AA13" s="28"/>
+      <c r="AB13" s="28"/>
+      <c r="AC13" s="28"/>
+      <c r="AD13" s="28"/>
+      <c r="AE13" s="28"/>
+      <c r="AF13" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="AI13" s="18"/>
-      <c r="AJ13" s="18"/>
-      <c r="AK13" s="18"/>
-      <c r="AL13" s="18"/>
-      <c r="AM13" s="18"/>
-      <c r="AN13" s="18"/>
-      <c r="AO13" s="18"/>
-      <c r="AP13" s="18"/>
-      <c r="AQ13" s="18"/>
-      <c r="AR13" s="18"/>
-      <c r="AS13" s="18" t="s">
+      <c r="AG13" s="28"/>
+      <c r="AH13" s="28"/>
+      <c r="AI13" s="28"/>
+      <c r="AJ13" s="28"/>
+      <c r="AK13" s="28"/>
+      <c r="AL13" s="28"/>
+      <c r="AM13" s="28"/>
+      <c r="AN13" s="28"/>
+      <c r="AO13" s="28"/>
+      <c r="AP13" s="28"/>
+      <c r="AQ13" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="AT13" s="18"/>
-      <c r="AU13" s="18"/>
-      <c r="AV13" s="18"/>
-      <c r="AW13" s="18"/>
-      <c r="AX13" s="18"/>
-      <c r="AY13" s="18"/>
-      <c r="AZ13" s="18"/>
-      <c r="BA13" s="18"/>
-      <c r="BB13" s="18"/>
-      <c r="BC13" s="18"/>
-      <c r="BD13" s="18" t="s">
+      <c r="AR13" s="28"/>
+      <c r="AS13" s="28"/>
+      <c r="AT13" s="28"/>
+      <c r="AU13" s="28"/>
+      <c r="AV13" s="28"/>
+      <c r="AW13" s="28"/>
+      <c r="AX13" s="28"/>
+      <c r="AY13" s="28"/>
+      <c r="AZ13" s="28"/>
+      <c r="BA13" s="28"/>
+      <c r="BB13" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="BE13" s="18"/>
-      <c r="BF13" s="18"/>
-      <c r="BG13" s="18"/>
-      <c r="BH13" s="18"/>
-      <c r="BI13" s="18"/>
-      <c r="BJ13" s="18"/>
-      <c r="BK13" s="18"/>
-      <c r="BL13" s="18"/>
-      <c r="BM13" s="18"/>
-      <c r="BN13" s="18"/>
-      <c r="BO13" s="18" t="s">
+      <c r="BC13" s="28"/>
+      <c r="BD13" s="28"/>
+      <c r="BE13" s="28"/>
+      <c r="BF13" s="28"/>
+      <c r="BG13" s="28"/>
+      <c r="BH13" s="28"/>
+      <c r="BI13" s="28"/>
+      <c r="BJ13" s="28"/>
+      <c r="BK13" s="28"/>
+      <c r="BL13" s="28"/>
+      <c r="BM13" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="BP13" s="18"/>
-      <c r="BQ13" s="18"/>
-      <c r="BR13" s="18"/>
-      <c r="BS13" s="18"/>
-      <c r="BT13" s="18"/>
-      <c r="BU13" s="18"/>
-      <c r="BV13" s="18"/>
-      <c r="BW13" s="18"/>
-      <c r="BX13" s="18"/>
-      <c r="BY13" s="18"/>
-      <c r="BZ13" s="18" t="s">
+      <c r="BN13" s="28"/>
+      <c r="BO13" s="28"/>
+      <c r="BP13" s="28"/>
+      <c r="BQ13" s="28"/>
+      <c r="BR13" s="28"/>
+      <c r="BS13" s="28"/>
+      <c r="BT13" s="28"/>
+      <c r="BU13" s="28"/>
+      <c r="BV13" s="28"/>
+      <c r="BW13" s="28"/>
+      <c r="BX13" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="CA13" s="18"/>
-      <c r="CB13" s="18"/>
-      <c r="CC13" s="18"/>
-      <c r="CD13" s="18"/>
-      <c r="CE13" s="18"/>
-      <c r="CF13" s="18"/>
-      <c r="CG13" s="18"/>
-      <c r="CH13" s="18"/>
-      <c r="CI13" s="18"/>
-      <c r="CJ13" s="18"/>
-      <c r="CK13" s="18" t="s">
+      <c r="BY13" s="28"/>
+      <c r="BZ13" s="28"/>
+      <c r="CA13" s="28"/>
+      <c r="CB13" s="28"/>
+      <c r="CC13" s="28"/>
+      <c r="CD13" s="28"/>
+      <c r="CE13" s="28"/>
+      <c r="CF13" s="28"/>
+      <c r="CG13" s="28"/>
+      <c r="CH13" s="28"/>
+      <c r="CI13" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="CL13" s="18"/>
-      <c r="CM13" s="18"/>
-      <c r="CN13" s="18"/>
-      <c r="CO13" s="18"/>
-      <c r="CP13" s="18"/>
-      <c r="CQ13" s="18"/>
-      <c r="CR13" s="18"/>
-      <c r="CS13" s="18"/>
-      <c r="CT13" s="18"/>
-      <c r="CU13" s="18"/>
-      <c r="CV13" s="18" t="s">
+      <c r="CJ13" s="28"/>
+      <c r="CK13" s="28"/>
+      <c r="CL13" s="28"/>
+      <c r="CM13" s="28"/>
+      <c r="CN13" s="28"/>
+      <c r="CO13" s="28"/>
+      <c r="CP13" s="28"/>
+      <c r="CQ13" s="28"/>
+      <c r="CR13" s="28"/>
+      <c r="CS13" s="28"/>
+      <c r="CT13" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="CW13" s="18"/>
-      <c r="CX13" s="18"/>
-      <c r="CY13" s="18"/>
-      <c r="CZ13" s="18"/>
-      <c r="DA13" s="18"/>
-      <c r="DB13" s="18"/>
-      <c r="DC13" s="18"/>
-      <c r="DD13" s="18"/>
-      <c r="DE13" s="18"/>
-      <c r="DF13" s="18"/>
-      <c r="DG13" s="18" t="s">
+      <c r="CU13" s="28"/>
+      <c r="CV13" s="28"/>
+      <c r="CW13" s="28"/>
+      <c r="CX13" s="28"/>
+      <c r="CY13" s="28"/>
+      <c r="CZ13" s="28"/>
+      <c r="DA13" s="28"/>
+      <c r="DB13" s="28"/>
+      <c r="DC13" s="28"/>
+      <c r="DD13" s="28"/>
+      <c r="DE13" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="DH13" s="18"/>
-      <c r="DI13" s="18"/>
-      <c r="DJ13" s="18"/>
-      <c r="DK13" s="18"/>
-      <c r="DL13" s="18"/>
-      <c r="DM13" s="18"/>
-      <c r="DN13" s="18"/>
-      <c r="DO13" s="18"/>
-      <c r="DP13" s="18"/>
-      <c r="DQ13" s="18"/>
-      <c r="DR13" s="22" t="s">
+      <c r="DF13" s="28"/>
+      <c r="DG13" s="28"/>
+      <c r="DH13" s="28"/>
+      <c r="DI13" s="28"/>
+      <c r="DJ13" s="28"/>
+      <c r="DK13" s="28"/>
+      <c r="DL13" s="28"/>
+      <c r="DM13" s="28"/>
+      <c r="DN13" s="28"/>
+      <c r="DO13" s="28"/>
+      <c r="DP13" s="25" t="s">
         <v>53</v>
       </c>
-      <c r="DS13" s="22" t="s">
+      <c r="DQ13" s="25" t="s">
         <v>54</v>
       </c>
-      <c r="DT13" s="22" t="s">
+      <c r="DR13" s="25" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="14" spans="1:126" x14ac:dyDescent="0.25">
-      <c r="A14" s="25"/>
-      <c r="B14" s="25"/>
-      <c r="C14" s="18" t="s">
+    <row r="14" spans="1:124" x14ac:dyDescent="0.25">
+      <c r="A14" s="21"/>
+      <c r="B14" s="21"/>
+      <c r="C14" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="D14" s="18" t="s">
+      <c r="D14" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="E14" s="18" t="s">
+      <c r="E14" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="F14" s="18" t="s">
+      <c r="F14" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="G14" s="21" t="s">
+      <c r="G14" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="H14" s="18" t="s">
+      <c r="H14" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="I14" s="18" t="s">
+      <c r="I14" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="J14" s="18" t="s">
+      <c r="J14" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="K14" s="25"/>
-      <c r="L14" s="18" t="s">
+      <c r="K14" s="21"/>
+      <c r="L14" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="M14" s="18" t="s">
+      <c r="M14" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="N14" s="18" t="s">
+      <c r="N14" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="O14" s="18" t="s">
+      <c r="O14" s="28" t="s">
         <v>42</v>
       </c>
-      <c r="P14" s="19" t="s">
+      <c r="P14" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="Q14" s="20"/>
-      <c r="R14" s="20"/>
-      <c r="S14" s="20"/>
-      <c r="T14" s="20"/>
-      <c r="U14" s="20"/>
-      <c r="V14" s="21"/>
-      <c r="W14" s="18" t="s">
+      <c r="Q14" s="23"/>
+      <c r="R14" s="23"/>
+      <c r="S14" s="23"/>
+      <c r="T14" s="24"/>
+      <c r="U14" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="X14" s="18" t="s">
+      <c r="V14" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="Y14" s="18" t="s">
+      <c r="W14" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="Z14" s="18" t="s">
+      <c r="X14" s="28" t="s">
         <v>42</v>
       </c>
-      <c r="AA14" s="19" t="s">
+      <c r="Y14" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="AB14" s="20"/>
-      <c r="AC14" s="20"/>
-      <c r="AD14" s="20"/>
-      <c r="AE14" s="20"/>
-      <c r="AF14" s="20"/>
-      <c r="AG14" s="21"/>
-      <c r="AH14" s="18" t="s">
+      <c r="Z14" s="23"/>
+      <c r="AA14" s="23"/>
+      <c r="AB14" s="23"/>
+      <c r="AC14" s="23"/>
+      <c r="AD14" s="23"/>
+      <c r="AE14" s="24"/>
+      <c r="AF14" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="AI14" s="18" t="s">
+      <c r="AG14" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="AJ14" s="18" t="s">
+      <c r="AH14" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="AK14" s="18" t="s">
+      <c r="AI14" s="28" t="s">
         <v>42</v>
       </c>
-      <c r="AL14" s="19" t="s">
+      <c r="AJ14" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="AM14" s="20"/>
-      <c r="AN14" s="20"/>
-      <c r="AO14" s="20"/>
-      <c r="AP14" s="20"/>
-      <c r="AQ14" s="20"/>
-      <c r="AR14" s="21"/>
-      <c r="AS14" s="18" t="s">
+      <c r="AK14" s="23"/>
+      <c r="AL14" s="23"/>
+      <c r="AM14" s="23"/>
+      <c r="AN14" s="23"/>
+      <c r="AO14" s="23"/>
+      <c r="AP14" s="24"/>
+      <c r="AQ14" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="AT14" s="18" t="s">
+      <c r="AR14" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="AU14" s="18" t="s">
+      <c r="AS14" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="AV14" s="18" t="s">
+      <c r="AT14" s="28" t="s">
         <v>42</v>
       </c>
-      <c r="AW14" s="19" t="s">
+      <c r="AU14" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="AX14" s="20"/>
-      <c r="AY14" s="20"/>
-      <c r="AZ14" s="20"/>
-      <c r="BA14" s="20"/>
-      <c r="BB14" s="20"/>
-      <c r="BC14" s="21"/>
-      <c r="BD14" s="18" t="s">
+      <c r="AV14" s="23"/>
+      <c r="AW14" s="23"/>
+      <c r="AX14" s="23"/>
+      <c r="AY14" s="23"/>
+      <c r="AZ14" s="23"/>
+      <c r="BA14" s="24"/>
+      <c r="BB14" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="BE14" s="18" t="s">
+      <c r="BC14" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="BF14" s="18" t="s">
+      <c r="BD14" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="BG14" s="18" t="s">
+      <c r="BE14" s="28" t="s">
         <v>42</v>
       </c>
-      <c r="BH14" s="19" t="s">
+      <c r="BF14" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="BI14" s="20"/>
-      <c r="BJ14" s="20"/>
-      <c r="BK14" s="20"/>
-      <c r="BL14" s="20"/>
-      <c r="BM14" s="20"/>
-      <c r="BN14" s="21"/>
-      <c r="BO14" s="18" t="s">
+      <c r="BG14" s="23"/>
+      <c r="BH14" s="23"/>
+      <c r="BI14" s="23"/>
+      <c r="BJ14" s="23"/>
+      <c r="BK14" s="23"/>
+      <c r="BL14" s="24"/>
+      <c r="BM14" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="BP14" s="18" t="s">
+      <c r="BN14" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="BQ14" s="18" t="s">
+      <c r="BO14" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="BR14" s="18" t="s">
+      <c r="BP14" s="28" t="s">
         <v>42</v>
       </c>
-      <c r="BS14" s="19" t="s">
+      <c r="BQ14" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="BT14" s="20"/>
-      <c r="BU14" s="20"/>
-      <c r="BV14" s="20"/>
-      <c r="BW14" s="20"/>
-      <c r="BX14" s="20"/>
-      <c r="BY14" s="21"/>
-      <c r="BZ14" s="18" t="s">
+      <c r="BR14" s="23"/>
+      <c r="BS14" s="23"/>
+      <c r="BT14" s="23"/>
+      <c r="BU14" s="23"/>
+      <c r="BV14" s="23"/>
+      <c r="BW14" s="24"/>
+      <c r="BX14" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="CA14" s="18" t="s">
+      <c r="BY14" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="CB14" s="18" t="s">
+      <c r="BZ14" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="CC14" s="18" t="s">
+      <c r="CA14" s="28" t="s">
         <v>42</v>
       </c>
-      <c r="CD14" s="19" t="s">
+      <c r="CB14" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="CE14" s="20"/>
-      <c r="CF14" s="20"/>
-      <c r="CG14" s="20"/>
-      <c r="CH14" s="20"/>
-      <c r="CI14" s="20"/>
-      <c r="CJ14" s="21"/>
-      <c r="CK14" s="18" t="s">
+      <c r="CC14" s="23"/>
+      <c r="CD14" s="23"/>
+      <c r="CE14" s="23"/>
+      <c r="CF14" s="23"/>
+      <c r="CG14" s="23"/>
+      <c r="CH14" s="24"/>
+      <c r="CI14" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="CL14" s="18" t="s">
+      <c r="CJ14" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="CM14" s="18" t="s">
+      <c r="CK14" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="CN14" s="18" t="s">
+      <c r="CL14" s="28" t="s">
         <v>42</v>
       </c>
-      <c r="CO14" s="19" t="s">
+      <c r="CM14" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="CP14" s="20"/>
-      <c r="CQ14" s="20"/>
-      <c r="CR14" s="20"/>
-      <c r="CS14" s="20"/>
-      <c r="CT14" s="20"/>
-      <c r="CU14" s="21"/>
-      <c r="CV14" s="18" t="s">
+      <c r="CN14" s="23"/>
+      <c r="CO14" s="23"/>
+      <c r="CP14" s="23"/>
+      <c r="CQ14" s="23"/>
+      <c r="CR14" s="23"/>
+      <c r="CS14" s="24"/>
+      <c r="CT14" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="CW14" s="18" t="s">
+      <c r="CU14" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="CX14" s="18" t="s">
+      <c r="CV14" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="CY14" s="18" t="s">
+      <c r="CW14" s="28" t="s">
         <v>42</v>
       </c>
-      <c r="CZ14" s="19" t="s">
+      <c r="CX14" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="DA14" s="20"/>
-      <c r="DB14" s="20"/>
-      <c r="DC14" s="20"/>
-      <c r="DD14" s="20"/>
-      <c r="DE14" s="20"/>
-      <c r="DF14" s="21"/>
-      <c r="DG14" s="18" t="s">
+      <c r="CY14" s="23"/>
+      <c r="CZ14" s="23"/>
+      <c r="DA14" s="23"/>
+      <c r="DB14" s="23"/>
+      <c r="DC14" s="23"/>
+      <c r="DD14" s="24"/>
+      <c r="DE14" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="DH14" s="18" t="s">
+      <c r="DF14" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="DI14" s="18" t="s">
+      <c r="DG14" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="DJ14" s="18" t="s">
+      <c r="DH14" s="28" t="s">
         <v>42</v>
       </c>
-      <c r="DK14" s="19" t="s">
+      <c r="DI14" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="DL14" s="20"/>
-      <c r="DM14" s="20"/>
-      <c r="DN14" s="20"/>
-      <c r="DO14" s="20"/>
-      <c r="DP14" s="20"/>
-      <c r="DQ14" s="21"/>
-      <c r="DR14" s="23"/>
-      <c r="DS14" s="23"/>
-      <c r="DT14" s="23"/>
+      <c r="DJ14" s="23"/>
+      <c r="DK14" s="23"/>
+      <c r="DL14" s="23"/>
+      <c r="DM14" s="23"/>
+      <c r="DN14" s="23"/>
+      <c r="DO14" s="24"/>
+      <c r="DP14" s="26"/>
+      <c r="DQ14" s="26"/>
+      <c r="DR14" s="26"/>
     </row>
-    <row r="15" spans="1:126" x14ac:dyDescent="0.25">
-      <c r="A15" s="25"/>
-      <c r="B15" s="25"/>
-      <c r="C15" s="18"/>
-      <c r="D15" s="18"/>
-      <c r="E15" s="18"/>
-      <c r="F15" s="18"/>
-      <c r="G15" s="18"/>
-      <c r="H15" s="18"/>
-      <c r="I15" s="18"/>
-      <c r="J15" s="18"/>
-      <c r="K15" s="25"/>
-      <c r="L15" s="18"/>
-      <c r="M15" s="18"/>
-      <c r="N15" s="18"/>
-      <c r="O15" s="18"/>
+    <row r="15" spans="1:124" x14ac:dyDescent="0.25">
+      <c r="A15" s="21"/>
+      <c r="B15" s="21"/>
+      <c r="C15" s="28"/>
+      <c r="D15" s="28"/>
+      <c r="E15" s="28"/>
+      <c r="F15" s="28"/>
+      <c r="G15" s="28"/>
+      <c r="H15" s="28"/>
+      <c r="I15" s="28"/>
+      <c r="J15" s="28"/>
+      <c r="K15" s="21"/>
+      <c r="L15" s="28"/>
+      <c r="M15" s="28"/>
+      <c r="N15" s="28"/>
+      <c r="O15" s="28"/>
       <c r="P15" s="12" t="s">
         <v>44</v>
       </c>
       <c r="Q15" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="R15" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="S15" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="T15" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="U15" s="28"/>
+      <c r="V15" s="28"/>
+      <c r="W15" s="28"/>
+      <c r="X15" s="28"/>
+      <c r="Y15" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="Z15" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="R15" s="12" t="s">
+      <c r="AA15" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="S15" s="12" t="s">
+      <c r="AB15" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="T15" s="12" t="s">
+      <c r="AC15" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="U15" s="12" t="s">
+      <c r="AD15" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="V15" s="12" t="s">
+      <c r="AE15" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="W15" s="18"/>
-      <c r="X15" s="18"/>
-      <c r="Y15" s="18"/>
-      <c r="Z15" s="18"/>
-      <c r="AA15" s="12" t="s">
+      <c r="AF15" s="28"/>
+      <c r="AG15" s="28"/>
+      <c r="AH15" s="28"/>
+      <c r="AI15" s="28"/>
+      <c r="AJ15" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="AB15" s="12" t="s">
+      <c r="AK15" s="12" t="s">
         <v>45</v>
       </c>
-      <c r="AC15" s="12" t="s">
+      <c r="AL15" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="AD15" s="12" t="s">
+      <c r="AM15" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="AE15" s="12" t="s">
+      <c r="AN15" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="AF15" s="12" t="s">
+      <c r="AO15" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="AG15" s="12" t="s">
+      <c r="AP15" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="AH15" s="18"/>
-      <c r="AI15" s="18"/>
-      <c r="AJ15" s="18"/>
-      <c r="AK15" s="18"/>
-      <c r="AL15" s="12" t="s">
+      <c r="AQ15" s="28"/>
+      <c r="AR15" s="28"/>
+      <c r="AS15" s="28"/>
+      <c r="AT15" s="28"/>
+      <c r="AU15" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="AM15" s="12" t="s">
+      <c r="AV15" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="AN15" s="12" t="s">
+      <c r="AW15" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="AO15" s="12" t="s">
+      <c r="AX15" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="AP15" s="12" t="s">
+      <c r="AY15" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="AQ15" s="12" t="s">
+      <c r="AZ15" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="AR15" s="12" t="s">
+      <c r="BA15" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="AS15" s="18"/>
-      <c r="AT15" s="18"/>
-      <c r="AU15" s="18"/>
-      <c r="AV15" s="18"/>
-      <c r="AW15" s="14" t="s">
+      <c r="BB15" s="28"/>
+      <c r="BC15" s="28"/>
+      <c r="BD15" s="28"/>
+      <c r="BE15" s="28"/>
+      <c r="BF15" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="AX15" s="14" t="s">
+      <c r="BG15" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="AY15" s="14" t="s">
+      <c r="BH15" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="AZ15" s="14" t="s">
+      <c r="BI15" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="BA15" s="14" t="s">
+      <c r="BJ15" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="BB15" s="14" t="s">
+      <c r="BK15" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="BC15" s="14" t="s">
+      <c r="BL15" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="BD15" s="18"/>
-      <c r="BE15" s="18"/>
-      <c r="BF15" s="18"/>
-      <c r="BG15" s="18"/>
-      <c r="BH15" s="14" t="s">
+      <c r="BM15" s="28"/>
+      <c r="BN15" s="28"/>
+      <c r="BO15" s="28"/>
+      <c r="BP15" s="28"/>
+      <c r="BQ15" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="BI15" s="14" t="s">
+      <c r="BR15" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="BJ15" s="14" t="s">
+      <c r="BS15" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="BK15" s="14" t="s">
+      <c r="BT15" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="BL15" s="14" t="s">
+      <c r="BU15" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="BM15" s="14" t="s">
+      <c r="BV15" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="BN15" s="14" t="s">
+      <c r="BW15" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="BO15" s="18"/>
-      <c r="BP15" s="18"/>
-      <c r="BQ15" s="18"/>
-      <c r="BR15" s="18"/>
-      <c r="BS15" s="14" t="s">
+      <c r="BX15" s="28"/>
+      <c r="BY15" s="28"/>
+      <c r="BZ15" s="28"/>
+      <c r="CA15" s="28"/>
+      <c r="CB15" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="BT15" s="14" t="s">
+      <c r="CC15" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="BU15" s="14" t="s">
+      <c r="CD15" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="BV15" s="14" t="s">
+      <c r="CE15" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="BW15" s="14" t="s">
+      <c r="CF15" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="BX15" s="14" t="s">
+      <c r="CG15" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="BY15" s="14" t="s">
+      <c r="CH15" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="BZ15" s="18"/>
-      <c r="CA15" s="18"/>
-      <c r="CB15" s="18"/>
-      <c r="CC15" s="18"/>
-      <c r="CD15" s="14" t="s">
+      <c r="CI15" s="28"/>
+      <c r="CJ15" s="28"/>
+      <c r="CK15" s="28"/>
+      <c r="CL15" s="28"/>
+      <c r="CM15" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="CE15" s="14" t="s">
+      <c r="CN15" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="CF15" s="14" t="s">
+      <c r="CO15" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="CG15" s="14" t="s">
+      <c r="CP15" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="CH15" s="14" t="s">
+      <c r="CQ15" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="CI15" s="14" t="s">
+      <c r="CR15" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="CJ15" s="14" t="s">
+      <c r="CS15" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="CK15" s="18"/>
-      <c r="CL15" s="18"/>
-      <c r="CM15" s="18"/>
-      <c r="CN15" s="18"/>
-      <c r="CO15" s="14" t="s">
+      <c r="CT15" s="28"/>
+      <c r="CU15" s="28"/>
+      <c r="CV15" s="28"/>
+      <c r="CW15" s="28"/>
+      <c r="CX15" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="CP15" s="14" t="s">
+      <c r="CY15" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="CQ15" s="14" t="s">
+      <c r="CZ15" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="CR15" s="14" t="s">
+      <c r="DA15" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="CS15" s="14" t="s">
+      <c r="DB15" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="CT15" s="14" t="s">
+      <c r="DC15" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="CU15" s="14" t="s">
+      <c r="DD15" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="CV15" s="18"/>
-      <c r="CW15" s="18"/>
-      <c r="CX15" s="18"/>
-      <c r="CY15" s="18"/>
-      <c r="CZ15" s="14" t="s">
+      <c r="DE15" s="28"/>
+      <c r="DF15" s="28"/>
+      <c r="DG15" s="28"/>
+      <c r="DH15" s="28"/>
+      <c r="DI15" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="DA15" s="14" t="s">
+      <c r="DJ15" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="DB15" s="14" t="s">
+      <c r="DK15" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="DC15" s="14" t="s">
+      <c r="DL15" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="DD15" s="14" t="s">
+      <c r="DM15" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="DE15" s="14" t="s">
+      <c r="DN15" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="DF15" s="14" t="s">
+      <c r="DO15" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="DG15" s="18"/>
-      <c r="DH15" s="18"/>
-      <c r="DI15" s="18"/>
-      <c r="DJ15" s="18"/>
-      <c r="DK15" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="DL15" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="DM15" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="DN15" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="DO15" s="14" t="s">
-        <v>48</v>
-      </c>
-      <c r="DP15" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="DQ15" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="DR15" s="24"/>
-      <c r="DS15" s="24"/>
-      <c r="DT15" s="24"/>
+      <c r="DP15" s="27"/>
+      <c r="DQ15" s="27"/>
+      <c r="DR15" s="27"/>
     </row>
-    <row r="16" spans="1:126" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:124" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="s">
         <v>38</v>
       </c>
@@ -2100,7 +2089,7 @@
       <c r="J16" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="K16" s="26" t="s">
+      <c r="K16" s="18" t="s">
         <v>41</v>
       </c>
       <c r="L16" s="11" t="s">
@@ -2119,369 +2108,367 @@
         <v>57</v>
       </c>
       <c r="Q16" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="R16" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="S16" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="T16" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="U16" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="V16" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="W16" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="X16" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="Y16" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="Z16" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="R16" s="11" t="s">
+      <c r="AA16" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="S16" s="11" t="s">
+      <c r="AB16" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="T16" s="11" t="s">
+      <c r="AC16" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="U16" s="11" t="s">
+      <c r="AD16" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="V16" s="11" t="s">
+      <c r="AE16" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="W16" s="11" t="s">
+      <c r="AF16" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="X16" s="11" t="s">
+      <c r="AG16" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="Y16" s="17" t="s">
+      <c r="AH16" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="Z16" s="11" t="s">
+      <c r="AI16" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="AA16" s="11" t="s">
+      <c r="AJ16" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="AB16" s="11" t="s">
+      <c r="AK16" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="AC16" s="11" t="s">
+      <c r="AL16" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="AD16" s="11" t="s">
+      <c r="AM16" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="AE16" s="11" t="s">
+      <c r="AN16" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="AF16" s="11" t="s">
+      <c r="AO16" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="AG16" s="11" t="s">
+      <c r="AP16" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="AH16" s="11" t="s">
+      <c r="AQ16" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="AI16" s="11" t="s">
+      <c r="AR16" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="AJ16" s="17" t="s">
+      <c r="AS16" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="AK16" s="11" t="s">
+      <c r="AT16" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="AL16" s="11" t="s">
+      <c r="AU16" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="AM16" s="11" t="s">
+      <c r="AV16" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="AN16" s="11" t="s">
+      <c r="AW16" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="AO16" s="11" t="s">
+      <c r="AX16" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="AP16" s="11" t="s">
+      <c r="AY16" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="AQ16" s="11" t="s">
+      <c r="AZ16" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="AR16" s="11" t="s">
+      <c r="BA16" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="AS16" s="11" t="s">
+      <c r="BB16" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="AT16" s="11" t="s">
+      <c r="BC16" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="AU16" s="17" t="s">
+      <c r="BD16" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="AV16" s="11" t="s">
+      <c r="BE16" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="AW16" s="11" t="s">
+      <c r="BF16" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="AX16" s="11" t="s">
+      <c r="BG16" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="AY16" s="11" t="s">
+      <c r="BH16" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="AZ16" s="11" t="s">
+      <c r="BI16" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="BA16" s="11" t="s">
+      <c r="BJ16" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="BB16" s="11" t="s">
+      <c r="BK16" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="BC16" s="11" t="s">
+      <c r="BL16" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="BD16" s="11" t="s">
+      <c r="BM16" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="BE16" s="11" t="s">
+      <c r="BN16" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="BF16" s="17" t="s">
+      <c r="BO16" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="BG16" s="11" t="s">
+      <c r="BP16" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="BH16" s="11" t="s">
+      <c r="BQ16" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="BI16" s="11" t="s">
+      <c r="BR16" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="BJ16" s="11" t="s">
+      <c r="BS16" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="BK16" s="11" t="s">
+      <c r="BT16" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="BL16" s="11" t="s">
+      <c r="BU16" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="BM16" s="11" t="s">
+      <c r="BV16" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="BN16" s="11" t="s">
+      <c r="BW16" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="BO16" s="11" t="s">
+      <c r="BX16" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="BP16" s="11" t="s">
+      <c r="BY16" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="BQ16" s="17" t="s">
+      <c r="BZ16" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="BR16" s="11" t="s">
+      <c r="CA16" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="BS16" s="11" t="s">
+      <c r="CB16" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="BT16" s="11" t="s">
+      <c r="CC16" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="BU16" s="11" t="s">
+      <c r="CD16" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="BV16" s="11" t="s">
+      <c r="CE16" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="BW16" s="11" t="s">
+      <c r="CF16" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="BX16" s="11" t="s">
+      <c r="CG16" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="BY16" s="11" t="s">
+      <c r="CH16" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="BZ16" s="11" t="s">
+      <c r="CI16" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="CA16" s="11" t="s">
+      <c r="CJ16" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="CB16" s="17" t="s">
+      <c r="CK16" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="CC16" s="11" t="s">
+      <c r="CL16" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="CD16" s="11" t="s">
+      <c r="CM16" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="CE16" s="11" t="s">
+      <c r="CN16" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="CF16" s="11" t="s">
+      <c r="CO16" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="CG16" s="11" t="s">
+      <c r="CP16" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="CH16" s="11" t="s">
+      <c r="CQ16" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="CI16" s="11" t="s">
+      <c r="CR16" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="CJ16" s="11" t="s">
+      <c r="CS16" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="CK16" s="11" t="s">
+      <c r="CT16" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="CL16" s="11" t="s">
+      <c r="CU16" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="CM16" s="17" t="s">
+      <c r="CV16" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="CN16" s="11" t="s">
+      <c r="CW16" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="CO16" s="11" t="s">
+      <c r="CX16" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="CP16" s="11" t="s">
+      <c r="CY16" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="CQ16" s="11" t="s">
+      <c r="CZ16" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="CR16" s="11" t="s">
+      <c r="DA16" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="CS16" s="11" t="s">
+      <c r="DB16" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="CT16" s="11" t="s">
+      <c r="DC16" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="CU16" s="11" t="s">
+      <c r="DD16" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="CV16" s="11" t="s">
+      <c r="DE16" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="CW16" s="11" t="s">
+      <c r="DF16" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="CX16" s="17" t="s">
+      <c r="DG16" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="CY16" s="11" t="s">
+      <c r="DH16" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="CZ16" s="11" t="s">
+      <c r="DI16" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="DA16" s="11" t="s">
+      <c r="DJ16" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="DB16" s="11" t="s">
+      <c r="DK16" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="DC16" s="11" t="s">
+      <c r="DL16" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="DD16" s="11" t="s">
+      <c r="DM16" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="DE16" s="11" t="s">
+      <c r="DN16" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="DF16" s="11" t="s">
+      <c r="DO16" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="DG16" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="DH16" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="DI16" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="DJ16" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="DK16" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="DL16" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="DM16" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="DN16" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="DO16" s="11" t="s">
-        <v>61</v>
-      </c>
       <c r="DP16" s="11" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="DQ16" s="11" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="DR16" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="DS16" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="DT16" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="DU16" s="13" t="s">
+      <c r="DS16" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="DV16" s="10"/>
+      <c r="DT16" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="77">
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="A13:A15"/>
-    <mergeCell ref="P14:V14"/>
-    <mergeCell ref="DR13:DR15"/>
-    <mergeCell ref="W13:AG13"/>
-    <mergeCell ref="AA14:AG14"/>
-    <mergeCell ref="AH13:AR13"/>
-    <mergeCell ref="AH14:AH15"/>
-    <mergeCell ref="AI14:AI15"/>
-    <mergeCell ref="AL14:AR14"/>
-    <mergeCell ref="Z14:Z15"/>
-    <mergeCell ref="Y14:Y15"/>
-    <mergeCell ref="X14:X15"/>
-    <mergeCell ref="B13:B15"/>
-    <mergeCell ref="K13:K15"/>
-    <mergeCell ref="C13:F13"/>
-    <mergeCell ref="G13:J13"/>
-    <mergeCell ref="DS13:DS15"/>
-    <mergeCell ref="DT13:DT15"/>
-    <mergeCell ref="AJ14:AJ15"/>
-    <mergeCell ref="AK14:AK15"/>
-    <mergeCell ref="L13:V13"/>
-    <mergeCell ref="L14:L15"/>
-    <mergeCell ref="M14:M15"/>
-    <mergeCell ref="N14:N15"/>
-    <mergeCell ref="O14:O15"/>
-    <mergeCell ref="W14:W15"/>
-    <mergeCell ref="BD13:BN13"/>
-    <mergeCell ref="BD14:BD15"/>
-    <mergeCell ref="BE14:BE15"/>
-    <mergeCell ref="BF14:BF15"/>
-    <mergeCell ref="BG14:BG15"/>
-    <mergeCell ref="BH14:BN14"/>
+    <mergeCell ref="DE13:DO13"/>
+    <mergeCell ref="DE14:DE15"/>
+    <mergeCell ref="DF14:DF15"/>
+    <mergeCell ref="DG14:DG15"/>
+    <mergeCell ref="DH14:DH15"/>
+    <mergeCell ref="DI14:DO14"/>
+    <mergeCell ref="CT13:DD13"/>
+    <mergeCell ref="CT14:CT15"/>
+    <mergeCell ref="CU14:CU15"/>
+    <mergeCell ref="CV14:CV15"/>
+    <mergeCell ref="CW14:CW15"/>
+    <mergeCell ref="CX14:DD14"/>
+    <mergeCell ref="CI13:CS13"/>
+    <mergeCell ref="CI14:CI15"/>
+    <mergeCell ref="CJ14:CJ15"/>
+    <mergeCell ref="CK14:CK15"/>
+    <mergeCell ref="CL14:CL15"/>
+    <mergeCell ref="CM14:CS14"/>
+    <mergeCell ref="BX13:CH13"/>
+    <mergeCell ref="BX14:BX15"/>
+    <mergeCell ref="BY14:BY15"/>
+    <mergeCell ref="BZ14:BZ15"/>
+    <mergeCell ref="CA14:CA15"/>
+    <mergeCell ref="CB14:CH14"/>
+    <mergeCell ref="BM13:BW13"/>
+    <mergeCell ref="BM14:BM15"/>
+    <mergeCell ref="BN14:BN15"/>
+    <mergeCell ref="BO14:BO15"/>
+    <mergeCell ref="BP14:BP15"/>
+    <mergeCell ref="BQ14:BW14"/>
+    <mergeCell ref="AQ13:BA13"/>
+    <mergeCell ref="AQ14:AQ15"/>
+    <mergeCell ref="AR14:AR15"/>
+    <mergeCell ref="AS14:AS15"/>
+    <mergeCell ref="AT14:AT15"/>
+    <mergeCell ref="AU14:BA14"/>
+    <mergeCell ref="BF14:BL14"/>
     <mergeCell ref="C14:C15"/>
     <mergeCell ref="D14:D15"/>
     <mergeCell ref="E14:E15"/>
@@ -2490,42 +2477,38 @@
     <mergeCell ref="H14:H15"/>
     <mergeCell ref="I14:I15"/>
     <mergeCell ref="J14:J15"/>
-    <mergeCell ref="AS13:BC13"/>
-    <mergeCell ref="AS14:AS15"/>
-    <mergeCell ref="AT14:AT15"/>
-    <mergeCell ref="AU14:AU15"/>
-    <mergeCell ref="AV14:AV15"/>
-    <mergeCell ref="AW14:BC14"/>
-    <mergeCell ref="BO13:BY13"/>
-    <mergeCell ref="BO14:BO15"/>
-    <mergeCell ref="BP14:BP15"/>
-    <mergeCell ref="BQ14:BQ15"/>
-    <mergeCell ref="BR14:BR15"/>
-    <mergeCell ref="BS14:BY14"/>
-    <mergeCell ref="BZ13:CJ13"/>
-    <mergeCell ref="BZ14:BZ15"/>
-    <mergeCell ref="CA14:CA15"/>
-    <mergeCell ref="CB14:CB15"/>
-    <mergeCell ref="CC14:CC15"/>
-    <mergeCell ref="CD14:CJ14"/>
-    <mergeCell ref="CK13:CU13"/>
-    <mergeCell ref="CK14:CK15"/>
-    <mergeCell ref="CL14:CL15"/>
-    <mergeCell ref="CM14:CM15"/>
-    <mergeCell ref="CN14:CN15"/>
-    <mergeCell ref="CO14:CU14"/>
-    <mergeCell ref="CV13:DF13"/>
-    <mergeCell ref="CV14:CV15"/>
-    <mergeCell ref="CW14:CW15"/>
-    <mergeCell ref="CX14:CX15"/>
-    <mergeCell ref="CY14:CY15"/>
-    <mergeCell ref="CZ14:DF14"/>
-    <mergeCell ref="DG13:DQ13"/>
-    <mergeCell ref="DG14:DG15"/>
-    <mergeCell ref="DH14:DH15"/>
-    <mergeCell ref="DI14:DI15"/>
-    <mergeCell ref="DJ14:DJ15"/>
-    <mergeCell ref="DK14:DQ14"/>
+    <mergeCell ref="G13:J13"/>
+    <mergeCell ref="DQ13:DQ15"/>
+    <mergeCell ref="DR13:DR15"/>
+    <mergeCell ref="AH14:AH15"/>
+    <mergeCell ref="AI14:AI15"/>
+    <mergeCell ref="L13:T13"/>
+    <mergeCell ref="L14:L15"/>
+    <mergeCell ref="M14:M15"/>
+    <mergeCell ref="N14:N15"/>
+    <mergeCell ref="O14:O15"/>
+    <mergeCell ref="U14:U15"/>
+    <mergeCell ref="BB13:BL13"/>
+    <mergeCell ref="BB14:BB15"/>
+    <mergeCell ref="BC14:BC15"/>
+    <mergeCell ref="BD14:BD15"/>
+    <mergeCell ref="BE14:BE15"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="A13:A15"/>
+    <mergeCell ref="P14:T14"/>
+    <mergeCell ref="DP13:DP15"/>
+    <mergeCell ref="U13:AE13"/>
+    <mergeCell ref="Y14:AE14"/>
+    <mergeCell ref="AF13:AP13"/>
+    <mergeCell ref="AF14:AF15"/>
+    <mergeCell ref="AG14:AG15"/>
+    <mergeCell ref="AJ14:AP14"/>
+    <mergeCell ref="X14:X15"/>
+    <mergeCell ref="W14:W15"/>
+    <mergeCell ref="V14:V15"/>
+    <mergeCell ref="B13:B15"/>
+    <mergeCell ref="K13:K15"/>
+    <mergeCell ref="C13:F13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
KIBON-1806 remove kindDubletten to increase performance
</commit_message>
<xml_diff>
--- a/ebegu-server/src/main/resources/reporting/Massenversand.xlsx
+++ b/ebegu-server/src/main/resources/reporting/Massenversand.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\IdeaProjects\ebegu\ebegu-server\src\main\resources\reporting\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\enja\IdeaProjects\ebegu2\ebegu-server\src\main\resources\reporting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{894825B1-B1E7-437C-B1AB-0A742F4CF43B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CE278DF-8EB8-4073-8CF8-4A77FA282B88}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="606" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="606" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="6" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="71">
   <si>
     <t>{auswertungVon}</t>
   </si>
@@ -445,7 +445,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -466,7 +466,7 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -877,7 +877,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:DA16"/>
+  <dimension ref="A1:CY16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
@@ -896,69 +896,69 @@
     <col min="11" max="11" width="11.140625" customWidth="1"/>
     <col min="12" max="12" width="10.140625" customWidth="1"/>
     <col min="13" max="13" width="18.140625"/>
-    <col min="16" max="16" width="19" customWidth="1"/>
-    <col min="17" max="17" width="25.85546875" customWidth="1"/>
-    <col min="18" max="18" width="17.42578125" customWidth="1"/>
-    <col min="19" max="19" width="24.28515625" customWidth="1"/>
-    <col min="20" max="20" width="11.140625" customWidth="1"/>
-    <col min="21" max="21" width="10.140625" customWidth="1"/>
-    <col min="25" max="25" width="23" customWidth="1"/>
-    <col min="26" max="26" width="25.85546875" customWidth="1"/>
-    <col min="27" max="27" width="17.42578125" customWidth="1"/>
-    <col min="28" max="28" width="24.28515625" customWidth="1"/>
-    <col min="29" max="29" width="11.140625" customWidth="1"/>
-    <col min="30" max="30" width="10.140625" customWidth="1"/>
-    <col min="34" max="34" width="23" customWidth="1"/>
-    <col min="35" max="35" width="25.85546875" customWidth="1"/>
-    <col min="36" max="36" width="17.42578125" customWidth="1"/>
-    <col min="37" max="37" width="24.28515625" customWidth="1"/>
-    <col min="38" max="38" width="11.140625" customWidth="1"/>
-    <col min="39" max="39" width="10.140625" customWidth="1"/>
-    <col min="43" max="43" width="23" customWidth="1"/>
-    <col min="44" max="44" width="25.85546875" customWidth="1"/>
-    <col min="45" max="45" width="17.42578125" customWidth="1"/>
-    <col min="46" max="46" width="24.28515625" customWidth="1"/>
-    <col min="47" max="47" width="11.140625" customWidth="1"/>
-    <col min="48" max="48" width="10.140625" customWidth="1"/>
-    <col min="52" max="52" width="23" customWidth="1"/>
-    <col min="53" max="53" width="25.85546875" customWidth="1"/>
-    <col min="54" max="54" width="17.42578125" customWidth="1"/>
-    <col min="55" max="55" width="24.28515625" customWidth="1"/>
-    <col min="56" max="56" width="11.140625" customWidth="1"/>
-    <col min="57" max="57" width="10.140625" customWidth="1"/>
-    <col min="61" max="61" width="23" customWidth="1"/>
-    <col min="62" max="62" width="25.85546875" customWidth="1"/>
-    <col min="63" max="63" width="17.42578125" customWidth="1"/>
-    <col min="64" max="64" width="24.28515625" customWidth="1"/>
-    <col min="65" max="65" width="11.140625" customWidth="1"/>
-    <col min="66" max="66" width="10.140625" customWidth="1"/>
-    <col min="70" max="70" width="23" customWidth="1"/>
-    <col min="71" max="71" width="25.85546875" customWidth="1"/>
-    <col min="72" max="72" width="17.42578125" customWidth="1"/>
-    <col min="73" max="73" width="24.28515625" customWidth="1"/>
-    <col min="74" max="74" width="11.140625" customWidth="1"/>
-    <col min="75" max="75" width="10.140625" customWidth="1"/>
-    <col min="79" max="79" width="23" customWidth="1"/>
-    <col min="80" max="80" width="25.85546875" customWidth="1"/>
-    <col min="81" max="81" width="17.42578125" customWidth="1"/>
-    <col min="82" max="82" width="24.28515625" customWidth="1"/>
-    <col min="83" max="83" width="11.140625" customWidth="1"/>
-    <col min="84" max="84" width="10.140625" customWidth="1"/>
-    <col min="88" max="88" width="23" customWidth="1"/>
-    <col min="89" max="89" width="25.85546875" customWidth="1"/>
-    <col min="90" max="90" width="17.42578125" customWidth="1"/>
-    <col min="91" max="91" width="24.28515625" customWidth="1"/>
-    <col min="92" max="92" width="11.140625" customWidth="1"/>
-    <col min="93" max="93" width="10.140625" customWidth="1"/>
-    <col min="97" max="97" width="23" customWidth="1"/>
-    <col min="98" max="98" width="25.85546875" customWidth="1"/>
-    <col min="99" max="99" width="17.42578125" customWidth="1"/>
-    <col min="100" max="102" width="24.28515625" customWidth="1"/>
-    <col min="103" max="103" width="15.7109375" customWidth="1"/>
-    <col min="104" max="1015" width="10.42578125"/>
+    <col min="15" max="15" width="19" customWidth="1"/>
+    <col min="16" max="16" width="25.85546875" customWidth="1"/>
+    <col min="17" max="17" width="17.42578125" customWidth="1"/>
+    <col min="18" max="18" width="24.28515625" customWidth="1"/>
+    <col min="19" max="19" width="11.140625" customWidth="1"/>
+    <col min="20" max="20" width="10.140625" customWidth="1"/>
+    <col min="23" max="23" width="23" customWidth="1"/>
+    <col min="24" max="24" width="25.85546875" customWidth="1"/>
+    <col min="25" max="25" width="17.42578125" customWidth="1"/>
+    <col min="26" max="26" width="24.28515625" customWidth="1"/>
+    <col min="27" max="27" width="11.140625" customWidth="1"/>
+    <col min="28" max="28" width="10.140625" customWidth="1"/>
+    <col min="32" max="32" width="23" customWidth="1"/>
+    <col min="33" max="33" width="25.85546875" customWidth="1"/>
+    <col min="34" max="34" width="17.42578125" customWidth="1"/>
+    <col min="35" max="35" width="24.28515625" customWidth="1"/>
+    <col min="36" max="36" width="11.140625" customWidth="1"/>
+    <col min="37" max="37" width="10.140625" customWidth="1"/>
+    <col min="41" max="41" width="23" customWidth="1"/>
+    <col min="42" max="42" width="25.85546875" customWidth="1"/>
+    <col min="43" max="43" width="17.42578125" customWidth="1"/>
+    <col min="44" max="44" width="24.28515625" customWidth="1"/>
+    <col min="45" max="45" width="11.140625" customWidth="1"/>
+    <col min="46" max="46" width="10.140625" customWidth="1"/>
+    <col min="50" max="50" width="23" customWidth="1"/>
+    <col min="51" max="51" width="25.85546875" customWidth="1"/>
+    <col min="52" max="52" width="17.42578125" customWidth="1"/>
+    <col min="53" max="53" width="24.28515625" customWidth="1"/>
+    <col min="54" max="54" width="11.140625" customWidth="1"/>
+    <col min="55" max="55" width="10.140625" customWidth="1"/>
+    <col min="59" max="59" width="23" customWidth="1"/>
+    <col min="60" max="60" width="25.85546875" customWidth="1"/>
+    <col min="61" max="61" width="17.42578125" customWidth="1"/>
+    <col min="62" max="62" width="24.28515625" customWidth="1"/>
+    <col min="63" max="63" width="11.140625" customWidth="1"/>
+    <col min="64" max="64" width="10.140625" customWidth="1"/>
+    <col min="68" max="68" width="23" customWidth="1"/>
+    <col min="69" max="69" width="25.85546875" customWidth="1"/>
+    <col min="70" max="70" width="17.42578125" customWidth="1"/>
+    <col min="71" max="71" width="24.28515625" customWidth="1"/>
+    <col min="72" max="72" width="11.140625" customWidth="1"/>
+    <col min="73" max="73" width="10.140625" customWidth="1"/>
+    <col min="77" max="77" width="23" customWidth="1"/>
+    <col min="78" max="78" width="25.85546875" customWidth="1"/>
+    <col min="79" max="79" width="17.42578125" customWidth="1"/>
+    <col min="80" max="80" width="24.28515625" customWidth="1"/>
+    <col min="81" max="81" width="11.140625" customWidth="1"/>
+    <col min="82" max="82" width="10.140625" customWidth="1"/>
+    <col min="86" max="86" width="23" customWidth="1"/>
+    <col min="87" max="87" width="25.85546875" customWidth="1"/>
+    <col min="88" max="88" width="17.42578125" customWidth="1"/>
+    <col min="89" max="89" width="24.28515625" customWidth="1"/>
+    <col min="90" max="90" width="11.140625" customWidth="1"/>
+    <col min="91" max="91" width="10.140625" customWidth="1"/>
+    <col min="95" max="95" width="23" customWidth="1"/>
+    <col min="96" max="96" width="25.85546875" customWidth="1"/>
+    <col min="97" max="97" width="17.42578125" customWidth="1"/>
+    <col min="98" max="100" width="24.28515625" customWidth="1"/>
+    <col min="101" max="101" width="15.7109375" customWidth="1"/>
+    <col min="102" max="1013" width="10.42578125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:105" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:103" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>31</v>
       </c>
@@ -969,10 +969,10 @@
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
     </row>
-    <row r="2" spans="1:105" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:103" x14ac:dyDescent="0.25">
       <c r="D2"/>
     </row>
-    <row r="3" spans="1:105" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:103" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>32</v>
       </c>
@@ -983,7 +983,7 @@
       <c r="F3" s="4"/>
       <c r="G3" s="4"/>
     </row>
-    <row r="4" spans="1:105" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:103" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>33</v>
       </c>
@@ -991,7 +991,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:105" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:103" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>34</v>
       </c>
@@ -999,7 +999,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:105" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:103" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>35</v>
       </c>
@@ -1007,7 +1007,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:105" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:103" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>37</v>
       </c>
@@ -1016,7 +1016,7 @@
       </c>
       <c r="C7" s="1"/>
     </row>
-    <row r="8" spans="1:105" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:103" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>38</v>
       </c>
@@ -1024,7 +1024,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:105" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:103" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>36</v>
       </c>
@@ -1032,7 +1032,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:105" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:103" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>39</v>
       </c>
@@ -1040,7 +1040,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:105" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:103" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>40</v>
       </c>
@@ -1051,7 +1051,7 @@
       <c r="E11" s="8"/>
       <c r="F11" s="8"/>
     </row>
-    <row r="12" spans="1:105" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:103" x14ac:dyDescent="0.25">
       <c r="D12"/>
       <c r="K12" t="s">
         <v>21</v>
@@ -1317,579 +1317,563 @@
       <c r="CT12" t="s">
         <v>21</v>
       </c>
-      <c r="CU12" t="s">
-        <v>21</v>
-      </c>
-      <c r="CV12" t="s">
-        <v>21</v>
-      </c>
     </row>
-    <row r="13" spans="1:105" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="21" t="s">
+    <row r="13" spans="1:103" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="B13" s="21" t="s">
+      <c r="B13" s="28" t="s">
         <v>69</v>
       </c>
-      <c r="C13" s="21" t="s">
+      <c r="C13" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="D13" s="28" t="s">
+      <c r="D13" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="E13" s="28"/>
-      <c r="F13" s="28"/>
-      <c r="G13" s="28" t="s">
+      <c r="E13" s="21"/>
+      <c r="F13" s="21"/>
+      <c r="G13" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="H13" s="28"/>
-      <c r="I13" s="28"/>
-      <c r="J13" s="21" t="s">
+      <c r="H13" s="21"/>
+      <c r="I13" s="21"/>
+      <c r="J13" s="28" t="s">
         <v>47</v>
       </c>
-      <c r="K13" s="28" t="s">
+      <c r="K13" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="L13" s="28"/>
-      <c r="M13" s="28"/>
-      <c r="N13" s="28"/>
-      <c r="O13" s="28"/>
-      <c r="P13" s="28"/>
-      <c r="Q13" s="28"/>
-      <c r="R13" s="28"/>
-      <c r="S13" s="28"/>
-      <c r="T13" s="28" t="s">
+      <c r="L13" s="21"/>
+      <c r="M13" s="21"/>
+      <c r="N13" s="21"/>
+      <c r="O13" s="21"/>
+      <c r="P13" s="21"/>
+      <c r="Q13" s="21"/>
+      <c r="R13" s="21"/>
+      <c r="S13" s="21" t="s">
         <v>57</v>
       </c>
-      <c r="U13" s="28"/>
-      <c r="V13" s="28"/>
-      <c r="W13" s="28"/>
-      <c r="X13" s="28"/>
-      <c r="Y13" s="28"/>
-      <c r="Z13" s="28"/>
-      <c r="AA13" s="28"/>
-      <c r="AB13" s="28"/>
-      <c r="AC13" s="28" t="s">
+      <c r="T13" s="21"/>
+      <c r="U13" s="21"/>
+      <c r="V13" s="21"/>
+      <c r="W13" s="21"/>
+      <c r="X13" s="21"/>
+      <c r="Y13" s="21"/>
+      <c r="Z13" s="21"/>
+      <c r="AA13" s="21" t="s">
         <v>58</v>
       </c>
-      <c r="AD13" s="28"/>
-      <c r="AE13" s="28"/>
-      <c r="AF13" s="28"/>
-      <c r="AG13" s="28"/>
-      <c r="AH13" s="28"/>
-      <c r="AI13" s="28"/>
-      <c r="AJ13" s="28"/>
-      <c r="AK13" s="28"/>
-      <c r="AL13" s="28" t="s">
+      <c r="AB13" s="21"/>
+      <c r="AC13" s="21"/>
+      <c r="AD13" s="21"/>
+      <c r="AE13" s="21"/>
+      <c r="AF13" s="21"/>
+      <c r="AG13" s="21"/>
+      <c r="AH13" s="21"/>
+      <c r="AI13" s="21"/>
+      <c r="AJ13" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="AM13" s="28"/>
-      <c r="AN13" s="28"/>
-      <c r="AO13" s="28"/>
-      <c r="AP13" s="28"/>
-      <c r="AQ13" s="28"/>
-      <c r="AR13" s="28"/>
-      <c r="AS13" s="28"/>
-      <c r="AT13" s="28"/>
-      <c r="AU13" s="28" t="s">
+      <c r="AK13" s="21"/>
+      <c r="AL13" s="21"/>
+      <c r="AM13" s="21"/>
+      <c r="AN13" s="21"/>
+      <c r="AO13" s="21"/>
+      <c r="AP13" s="21"/>
+      <c r="AQ13" s="21"/>
+      <c r="AR13" s="21"/>
+      <c r="AS13" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="AV13" s="28"/>
-      <c r="AW13" s="28"/>
-      <c r="AX13" s="28"/>
-      <c r="AY13" s="28"/>
-      <c r="AZ13" s="28"/>
-      <c r="BA13" s="28"/>
-      <c r="BB13" s="28"/>
-      <c r="BC13" s="28"/>
-      <c r="BD13" s="28" t="s">
+      <c r="AT13" s="21"/>
+      <c r="AU13" s="21"/>
+      <c r="AV13" s="21"/>
+      <c r="AW13" s="21"/>
+      <c r="AX13" s="21"/>
+      <c r="AY13" s="21"/>
+      <c r="AZ13" s="21"/>
+      <c r="BA13" s="21"/>
+      <c r="BB13" s="21" t="s">
         <v>61</v>
       </c>
-      <c r="BE13" s="28"/>
-      <c r="BF13" s="28"/>
-      <c r="BG13" s="28"/>
-      <c r="BH13" s="28"/>
-      <c r="BI13" s="28"/>
-      <c r="BJ13" s="28"/>
-      <c r="BK13" s="28"/>
-      <c r="BL13" s="28"/>
-      <c r="BM13" s="28" t="s">
+      <c r="BC13" s="21"/>
+      <c r="BD13" s="21"/>
+      <c r="BE13" s="21"/>
+      <c r="BF13" s="21"/>
+      <c r="BG13" s="21"/>
+      <c r="BH13" s="21"/>
+      <c r="BI13" s="21"/>
+      <c r="BJ13" s="21"/>
+      <c r="BK13" s="21" t="s">
         <v>62</v>
       </c>
-      <c r="BN13" s="28"/>
-      <c r="BO13" s="28"/>
-      <c r="BP13" s="28"/>
-      <c r="BQ13" s="28"/>
-      <c r="BR13" s="28"/>
-      <c r="BS13" s="28"/>
-      <c r="BT13" s="28"/>
-      <c r="BU13" s="28"/>
-      <c r="BV13" s="28" t="s">
+      <c r="BL13" s="21"/>
+      <c r="BM13" s="21"/>
+      <c r="BN13" s="21"/>
+      <c r="BO13" s="21"/>
+      <c r="BP13" s="21"/>
+      <c r="BQ13" s="21"/>
+      <c r="BR13" s="21"/>
+      <c r="BS13" s="21"/>
+      <c r="BT13" s="21" t="s">
         <v>63</v>
       </c>
-      <c r="BW13" s="28"/>
-      <c r="BX13" s="28"/>
-      <c r="BY13" s="28"/>
-      <c r="BZ13" s="28"/>
-      <c r="CA13" s="28"/>
-      <c r="CB13" s="28"/>
-      <c r="CC13" s="28"/>
-      <c r="CD13" s="28"/>
-      <c r="CE13" s="28" t="s">
+      <c r="BU13" s="21"/>
+      <c r="BV13" s="21"/>
+      <c r="BW13" s="21"/>
+      <c r="BX13" s="21"/>
+      <c r="BY13" s="21"/>
+      <c r="BZ13" s="21"/>
+      <c r="CA13" s="21"/>
+      <c r="CB13" s="21"/>
+      <c r="CC13" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="CF13" s="28"/>
-      <c r="CG13" s="28"/>
-      <c r="CH13" s="28"/>
-      <c r="CI13" s="28"/>
-      <c r="CJ13" s="28"/>
-      <c r="CK13" s="28"/>
-      <c r="CL13" s="28"/>
-      <c r="CM13" s="28"/>
-      <c r="CN13" s="28" t="s">
+      <c r="CD13" s="21"/>
+      <c r="CE13" s="21"/>
+      <c r="CF13" s="21"/>
+      <c r="CG13" s="21"/>
+      <c r="CH13" s="21"/>
+      <c r="CI13" s="21"/>
+      <c r="CJ13" s="21"/>
+      <c r="CK13" s="21"/>
+      <c r="CL13" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="CO13" s="28"/>
-      <c r="CP13" s="28"/>
-      <c r="CQ13" s="28"/>
-      <c r="CR13" s="28"/>
-      <c r="CS13" s="28"/>
-      <c r="CT13" s="28"/>
-      <c r="CU13" s="28"/>
-      <c r="CV13" s="28"/>
+      <c r="CM13" s="21"/>
+      <c r="CN13" s="21"/>
+      <c r="CO13" s="21"/>
+      <c r="CP13" s="21"/>
+      <c r="CQ13" s="21"/>
+      <c r="CR13" s="21"/>
+      <c r="CS13" s="21"/>
+      <c r="CT13" s="21"/>
+      <c r="CU13" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="CV13" s="25" t="s">
+        <v>67</v>
+      </c>
       <c r="CW13" s="25" t="s">
-        <v>66</v>
-      </c>
-      <c r="CX13" s="25" t="s">
-        <v>67</v>
-      </c>
-      <c r="CY13" s="25" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="14" spans="1:105" x14ac:dyDescent="0.25">
-      <c r="A14" s="21"/>
-      <c r="B14" s="21"/>
-      <c r="C14" s="21"/>
-      <c r="D14" s="28" t="s">
+    <row r="14" spans="1:103" x14ac:dyDescent="0.25">
+      <c r="A14" s="28"/>
+      <c r="B14" s="28"/>
+      <c r="C14" s="28"/>
+      <c r="D14" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="E14" s="28" t="s">
+      <c r="E14" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="F14" s="28" t="s">
+      <c r="F14" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="G14" s="28" t="s">
+      <c r="G14" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="H14" s="28" t="s">
+      <c r="H14" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="I14" s="28" t="s">
+      <c r="I14" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="J14" s="21"/>
-      <c r="K14" s="28" t="s">
+      <c r="J14" s="28"/>
+      <c r="K14" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="L14" s="28" t="s">
+      <c r="L14" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="M14" s="28" t="s">
+      <c r="M14" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="N14" s="28" t="s">
-        <v>49</v>
-      </c>
-      <c r="O14" s="22" t="s">
+      <c r="N14" s="22" t="s">
         <v>51</v>
       </c>
+      <c r="O14" s="23"/>
       <c r="P14" s="23"/>
       <c r="Q14" s="23"/>
-      <c r="R14" s="23"/>
-      <c r="S14" s="24"/>
-      <c r="T14" s="28" t="s">
+      <c r="R14" s="24"/>
+      <c r="S14" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="U14" s="28" t="s">
+      <c r="T14" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="V14" s="28" t="s">
+      <c r="U14" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="W14" s="28" t="s">
+      <c r="V14" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="W14" s="23"/>
+      <c r="X14" s="23"/>
+      <c r="Y14" s="23"/>
+      <c r="Z14" s="24"/>
+      <c r="AA14" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="AB14" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="AC14" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="AD14" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="X14" s="22" t="s">
+      <c r="AE14" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="Y14" s="23"/>
-      <c r="Z14" s="23"/>
-      <c r="AA14" s="23"/>
-      <c r="AB14" s="24"/>
-      <c r="AC14" s="28" t="s">
+      <c r="AF14" s="23"/>
+      <c r="AG14" s="23"/>
+      <c r="AH14" s="23"/>
+      <c r="AI14" s="24"/>
+      <c r="AJ14" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="AD14" s="28" t="s">
+      <c r="AK14" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="AE14" s="28" t="s">
+      <c r="AL14" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="AF14" s="28" t="s">
+      <c r="AM14" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="AG14" s="22" t="s">
+      <c r="AN14" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="AH14" s="23"/>
-      <c r="AI14" s="23"/>
-      <c r="AJ14" s="23"/>
-      <c r="AK14" s="24"/>
-      <c r="AL14" s="28" t="s">
+      <c r="AO14" s="23"/>
+      <c r="AP14" s="23"/>
+      <c r="AQ14" s="23"/>
+      <c r="AR14" s="24"/>
+      <c r="AS14" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="AM14" s="28" t="s">
+      <c r="AT14" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="AN14" s="28" t="s">
+      <c r="AU14" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="AO14" s="28" t="s">
+      <c r="AV14" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="AP14" s="22" t="s">
+      <c r="AW14" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="AQ14" s="23"/>
-      <c r="AR14" s="23"/>
-      <c r="AS14" s="23"/>
-      <c r="AT14" s="24"/>
-      <c r="AU14" s="28" t="s">
+      <c r="AX14" s="23"/>
+      <c r="AY14" s="23"/>
+      <c r="AZ14" s="23"/>
+      <c r="BA14" s="24"/>
+      <c r="BB14" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="AV14" s="28" t="s">
+      <c r="BC14" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="AW14" s="28" t="s">
+      <c r="BD14" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="AX14" s="28" t="s">
+      <c r="BE14" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="AY14" s="22" t="s">
+      <c r="BF14" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="AZ14" s="23"/>
-      <c r="BA14" s="23"/>
-      <c r="BB14" s="23"/>
-      <c r="BC14" s="24"/>
-      <c r="BD14" s="28" t="s">
+      <c r="BG14" s="23"/>
+      <c r="BH14" s="23"/>
+      <c r="BI14" s="23"/>
+      <c r="BJ14" s="24"/>
+      <c r="BK14" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="BE14" s="28" t="s">
+      <c r="BL14" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="BF14" s="28" t="s">
+      <c r="BM14" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="BG14" s="28" t="s">
+      <c r="BN14" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="BH14" s="22" t="s">
+      <c r="BO14" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="BI14" s="23"/>
-      <c r="BJ14" s="23"/>
-      <c r="BK14" s="23"/>
-      <c r="BL14" s="24"/>
-      <c r="BM14" s="28" t="s">
+      <c r="BP14" s="23"/>
+      <c r="BQ14" s="23"/>
+      <c r="BR14" s="23"/>
+      <c r="BS14" s="24"/>
+      <c r="BT14" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="BN14" s="28" t="s">
+      <c r="BU14" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="BO14" s="28" t="s">
+      <c r="BV14" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="BP14" s="28" t="s">
+      <c r="BW14" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="BQ14" s="22" t="s">
+      <c r="BX14" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="BR14" s="23"/>
-      <c r="BS14" s="23"/>
-      <c r="BT14" s="23"/>
-      <c r="BU14" s="24"/>
-      <c r="BV14" s="28" t="s">
+      <c r="BY14" s="23"/>
+      <c r="BZ14" s="23"/>
+      <c r="CA14" s="23"/>
+      <c r="CB14" s="24"/>
+      <c r="CC14" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="BW14" s="28" t="s">
+      <c r="CD14" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="BX14" s="28" t="s">
+      <c r="CE14" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="BY14" s="28" t="s">
+      <c r="CF14" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="BZ14" s="22" t="s">
+      <c r="CG14" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="CA14" s="23"/>
-      <c r="CB14" s="23"/>
-      <c r="CC14" s="23"/>
-      <c r="CD14" s="24"/>
-      <c r="CE14" s="28" t="s">
+      <c r="CH14" s="23"/>
+      <c r="CI14" s="23"/>
+      <c r="CJ14" s="23"/>
+      <c r="CK14" s="24"/>
+      <c r="CL14" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="CF14" s="28" t="s">
+      <c r="CM14" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="CG14" s="28" t="s">
+      <c r="CN14" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="CH14" s="28" t="s">
+      <c r="CO14" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="CI14" s="22" t="s">
+      <c r="CP14" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="CJ14" s="23"/>
-      <c r="CK14" s="23"/>
-      <c r="CL14" s="23"/>
-      <c r="CM14" s="24"/>
-      <c r="CN14" s="28" t="s">
-        <v>44</v>
-      </c>
-      <c r="CO14" s="28" t="s">
-        <v>45</v>
-      </c>
-      <c r="CP14" s="28" t="s">
-        <v>48</v>
-      </c>
-      <c r="CQ14" s="28" t="s">
-        <v>49</v>
-      </c>
-      <c r="CR14" s="22" t="s">
-        <v>51</v>
-      </c>
+      <c r="CQ14" s="23"/>
+      <c r="CR14" s="23"/>
       <c r="CS14" s="23"/>
-      <c r="CT14" s="23"/>
-      <c r="CU14" s="23"/>
-      <c r="CV14" s="24"/>
+      <c r="CT14" s="24"/>
+      <c r="CU14" s="26"/>
+      <c r="CV14" s="26"/>
       <c r="CW14" s="26"/>
-      <c r="CX14" s="26"/>
-      <c r="CY14" s="26"/>
     </row>
-    <row r="15" spans="1:105" x14ac:dyDescent="0.25">
-      <c r="A15" s="21"/>
-      <c r="B15" s="21"/>
-      <c r="C15" s="21"/>
-      <c r="D15" s="28"/>
-      <c r="E15" s="28"/>
-      <c r="F15" s="28"/>
-      <c r="G15" s="28"/>
-      <c r="H15" s="28"/>
-      <c r="I15" s="28"/>
-      <c r="J15" s="21"/>
-      <c r="K15" s="28"/>
-      <c r="L15" s="28"/>
-      <c r="M15" s="28"/>
-      <c r="N15" s="28"/>
+    <row r="15" spans="1:103" x14ac:dyDescent="0.25">
+      <c r="A15" s="28"/>
+      <c r="B15" s="28"/>
+      <c r="C15" s="28"/>
+      <c r="D15" s="21"/>
+      <c r="E15" s="21"/>
+      <c r="F15" s="21"/>
+      <c r="G15" s="21"/>
+      <c r="H15" s="21"/>
+      <c r="I15" s="21"/>
+      <c r="J15" s="28"/>
+      <c r="K15" s="21"/>
+      <c r="L15" s="21"/>
+      <c r="M15" s="21"/>
+      <c r="N15" s="12" t="s">
+        <v>52</v>
+      </c>
       <c r="O15" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="P15" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q15" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="R15" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="S15" s="21"/>
+      <c r="T15" s="21"/>
+      <c r="U15" s="21"/>
+      <c r="V15" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="P15" s="12" t="s">
+      <c r="W15" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="Q15" s="12" t="s">
+      <c r="X15" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="R15" s="12" t="s">
+      <c r="Y15" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="S15" s="12" t="s">
+      <c r="Z15" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="T15" s="28"/>
-      <c r="U15" s="28"/>
-      <c r="V15" s="28"/>
-      <c r="W15" s="28"/>
-      <c r="X15" s="18" t="s">
+      <c r="AA15" s="21"/>
+      <c r="AB15" s="21"/>
+      <c r="AC15" s="21"/>
+      <c r="AD15" s="21"/>
+      <c r="AE15" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="Y15" s="18" t="s">
+      <c r="AF15" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="Z15" s="18" t="s">
+      <c r="AG15" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="AA15" s="18" t="s">
+      <c r="AH15" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="AB15" s="18" t="s">
+      <c r="AI15" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="AC15" s="28"/>
-      <c r="AD15" s="28"/>
-      <c r="AE15" s="28"/>
-      <c r="AF15" s="28"/>
-      <c r="AG15" s="18" t="s">
+      <c r="AJ15" s="21"/>
+      <c r="AK15" s="21"/>
+      <c r="AL15" s="21"/>
+      <c r="AM15" s="21"/>
+      <c r="AN15" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="AH15" s="18" t="s">
+      <c r="AO15" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="AI15" s="18" t="s">
+      <c r="AP15" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="AJ15" s="18" t="s">
+      <c r="AQ15" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="AK15" s="18" t="s">
+      <c r="AR15" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="AL15" s="28"/>
-      <c r="AM15" s="28"/>
-      <c r="AN15" s="28"/>
-      <c r="AO15" s="28"/>
-      <c r="AP15" s="18" t="s">
+      <c r="AS15" s="21"/>
+      <c r="AT15" s="21"/>
+      <c r="AU15" s="21"/>
+      <c r="AV15" s="21"/>
+      <c r="AW15" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="AQ15" s="18" t="s">
+      <c r="AX15" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="AR15" s="18" t="s">
+      <c r="AY15" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="AS15" s="18" t="s">
+      <c r="AZ15" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="AT15" s="18" t="s">
+      <c r="BA15" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="AU15" s="28"/>
-      <c r="AV15" s="28"/>
-      <c r="AW15" s="28"/>
-      <c r="AX15" s="28"/>
-      <c r="AY15" s="18" t="s">
+      <c r="BB15" s="21"/>
+      <c r="BC15" s="21"/>
+      <c r="BD15" s="21"/>
+      <c r="BE15" s="21"/>
+      <c r="BF15" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="AZ15" s="18" t="s">
+      <c r="BG15" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="BA15" s="18" t="s">
+      <c r="BH15" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="BB15" s="18" t="s">
+      <c r="BI15" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="BC15" s="18" t="s">
+      <c r="BJ15" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="BD15" s="28"/>
-      <c r="BE15" s="28"/>
-      <c r="BF15" s="28"/>
-      <c r="BG15" s="28"/>
-      <c r="BH15" s="18" t="s">
+      <c r="BK15" s="21"/>
+      <c r="BL15" s="21"/>
+      <c r="BM15" s="21"/>
+      <c r="BN15" s="21"/>
+      <c r="BO15" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="BI15" s="18" t="s">
+      <c r="BP15" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="BJ15" s="18" t="s">
+      <c r="BQ15" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="BK15" s="18" t="s">
+      <c r="BR15" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="BL15" s="18" t="s">
+      <c r="BS15" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="BM15" s="28"/>
-      <c r="BN15" s="28"/>
-      <c r="BO15" s="28"/>
-      <c r="BP15" s="28"/>
-      <c r="BQ15" s="18" t="s">
+      <c r="BT15" s="21"/>
+      <c r="BU15" s="21"/>
+      <c r="BV15" s="21"/>
+      <c r="BW15" s="21"/>
+      <c r="BX15" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="BR15" s="18" t="s">
+      <c r="BY15" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="BS15" s="18" t="s">
+      <c r="BZ15" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="BT15" s="18" t="s">
+      <c r="CA15" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="BU15" s="18" t="s">
+      <c r="CB15" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="BV15" s="28"/>
-      <c r="BW15" s="28"/>
-      <c r="BX15" s="28"/>
-      <c r="BY15" s="28"/>
-      <c r="BZ15" s="18" t="s">
+      <c r="CC15" s="21"/>
+      <c r="CD15" s="21"/>
+      <c r="CE15" s="21"/>
+      <c r="CF15" s="21"/>
+      <c r="CG15" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="CA15" s="18" t="s">
+      <c r="CH15" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="CB15" s="18" t="s">
+      <c r="CI15" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="CC15" s="18" t="s">
+      <c r="CJ15" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="CD15" s="18" t="s">
+      <c r="CK15" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="CE15" s="28"/>
-      <c r="CF15" s="28"/>
-      <c r="CG15" s="28"/>
-      <c r="CH15" s="28"/>
-      <c r="CI15" s="18" t="s">
+      <c r="CL15" s="21"/>
+      <c r="CM15" s="21"/>
+      <c r="CN15" s="21"/>
+      <c r="CO15" s="21"/>
+      <c r="CP15" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="CJ15" s="18" t="s">
+      <c r="CQ15" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="CK15" s="18" t="s">
+      <c r="CR15" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="CL15" s="18" t="s">
+      <c r="CS15" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="CM15" s="18" t="s">
+      <c r="CT15" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="CN15" s="28"/>
-      <c r="CO15" s="28"/>
-      <c r="CP15" s="28"/>
-      <c r="CQ15" s="28"/>
-      <c r="CR15" s="18" t="s">
-        <v>52</v>
-      </c>
-      <c r="CS15" s="18" t="s">
-        <v>54</v>
-      </c>
-      <c r="CT15" s="18" t="s">
-        <v>55</v>
-      </c>
-      <c r="CU15" s="18" t="s">
-        <v>53</v>
-      </c>
-      <c r="CV15" s="18" t="s">
-        <v>56</v>
-      </c>
+      <c r="CU15" s="27"/>
+      <c r="CV15" s="27"/>
       <c r="CW15" s="27"/>
-      <c r="CX15" s="27"/>
-      <c r="CY15" s="27"/>
     </row>
-    <row r="16" spans="1:105" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:103" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="s">
         <v>18</v>
       </c>
@@ -1930,357 +1914,349 @@
         <v>9</v>
       </c>
       <c r="N16" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="O16" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="P16" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q16" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="R16" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="S16" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="T16" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="U16" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="V16" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="W16" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="X16" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y16" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="Z16" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="AA16" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="AB16" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="AC16" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="AD16" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="O16" s="11" t="s">
+      <c r="AE16" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="P16" s="11" t="s">
+      <c r="AF16" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="Q16" s="11" t="s">
+      <c r="AG16" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="R16" s="11" t="s">
+      <c r="AH16" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="S16" s="11" t="s">
+      <c r="AI16" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="T16" s="11" t="s">
+      <c r="AJ16" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="U16" s="11" t="s">
+      <c r="AK16" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="V16" s="16" t="s">
+      <c r="AL16" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="W16" s="11" t="s">
+      <c r="AM16" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="X16" s="11" t="s">
+      <c r="AN16" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="Y16" s="11" t="s">
+      <c r="AO16" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="Z16" s="11" t="s">
+      <c r="AP16" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="AA16" s="11" t="s">
+      <c r="AQ16" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="AB16" s="11" t="s">
+      <c r="AR16" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="AC16" s="11" t="s">
+      <c r="AS16" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="AD16" s="11" t="s">
+      <c r="AT16" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="AE16" s="16" t="s">
+      <c r="AU16" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="AF16" s="11" t="s">
+      <c r="AV16" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="AG16" s="11" t="s">
+      <c r="AW16" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="AH16" s="11" t="s">
+      <c r="AX16" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="AI16" s="11" t="s">
+      <c r="AY16" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="AJ16" s="11" t="s">
+      <c r="AZ16" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="AK16" s="11" t="s">
+      <c r="BA16" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="AL16" s="11" t="s">
+      <c r="BB16" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="AM16" s="11" t="s">
+      <c r="BC16" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="AN16" s="16" t="s">
+      <c r="BD16" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="AO16" s="11" t="s">
+      <c r="BE16" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="AP16" s="11" t="s">
+      <c r="BF16" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="AQ16" s="11" t="s">
+      <c r="BG16" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="AR16" s="11" t="s">
+      <c r="BH16" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="AS16" s="11" t="s">
+      <c r="BI16" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="AT16" s="11" t="s">
+      <c r="BJ16" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="AU16" s="11" t="s">
+      <c r="BK16" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="AV16" s="11" t="s">
+      <c r="BL16" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="AW16" s="16" t="s">
+      <c r="BM16" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="AX16" s="11" t="s">
+      <c r="BN16" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="AY16" s="11" t="s">
+      <c r="BO16" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="AZ16" s="11" t="s">
+      <c r="BP16" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="BA16" s="11" t="s">
+      <c r="BQ16" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="BB16" s="11" t="s">
+      <c r="BR16" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="BC16" s="11" t="s">
+      <c r="BS16" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="BD16" s="11" t="s">
+      <c r="BT16" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="BE16" s="11" t="s">
+      <c r="BU16" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="BF16" s="16" t="s">
+      <c r="BV16" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="BG16" s="11" t="s">
+      <c r="BW16" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="BH16" s="11" t="s">
+      <c r="BX16" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="BI16" s="11" t="s">
+      <c r="BY16" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="BJ16" s="11" t="s">
+      <c r="BZ16" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="BK16" s="11" t="s">
+      <c r="CA16" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="BL16" s="11" t="s">
+      <c r="CB16" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="BM16" s="11" t="s">
+      <c r="CC16" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="BN16" s="11" t="s">
+      <c r="CD16" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="BO16" s="16" t="s">
+      <c r="CE16" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="BP16" s="11" t="s">
+      <c r="CF16" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="BQ16" s="11" t="s">
+      <c r="CG16" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="BR16" s="11" t="s">
+      <c r="CH16" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="BS16" s="11" t="s">
+      <c r="CI16" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="BT16" s="11" t="s">
+      <c r="CJ16" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="BU16" s="11" t="s">
+      <c r="CK16" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="BV16" s="11" t="s">
+      <c r="CL16" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="BW16" s="11" t="s">
+      <c r="CM16" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="BX16" s="16" t="s">
+      <c r="CN16" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="BY16" s="11" t="s">
+      <c r="CO16" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="BZ16" s="11" t="s">
+      <c r="CP16" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="CA16" s="11" t="s">
+      <c r="CQ16" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="CB16" s="11" t="s">
+      <c r="CR16" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="CC16" s="11" t="s">
+      <c r="CS16" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="CD16" s="11" t="s">
+      <c r="CT16" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="CE16" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="CF16" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="CG16" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="CH16" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="CI16" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="CJ16" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="CK16" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="CL16" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="CM16" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="CN16" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="CO16" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="CP16" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="CQ16" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="CR16" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="CS16" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="CT16" s="11" t="s">
-        <v>24</v>
-      </c>
       <c r="CU16" s="11" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="CV16" s="11" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="CW16" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="CX16" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="CY16" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="CZ16" s="13" t="s">
+      <c r="CX16" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="DA16" s="10"/>
+      <c r="CY16" s="10"/>
     </row>
   </sheetData>
-  <mergeCells count="75">
-    <mergeCell ref="CN13:CV13"/>
-    <mergeCell ref="CN14:CN15"/>
-    <mergeCell ref="CO14:CO15"/>
-    <mergeCell ref="CP14:CP15"/>
-    <mergeCell ref="CQ14:CQ15"/>
-    <mergeCell ref="CR14:CV14"/>
-    <mergeCell ref="CE13:CM13"/>
-    <mergeCell ref="CE14:CE15"/>
-    <mergeCell ref="CF14:CF15"/>
-    <mergeCell ref="CG14:CG15"/>
-    <mergeCell ref="CH14:CH15"/>
-    <mergeCell ref="CI14:CM14"/>
-    <mergeCell ref="BV13:CD13"/>
-    <mergeCell ref="BV14:BV15"/>
-    <mergeCell ref="BW14:BW15"/>
-    <mergeCell ref="BX14:BX15"/>
-    <mergeCell ref="BY14:BY15"/>
-    <mergeCell ref="BZ14:CD14"/>
-    <mergeCell ref="BM13:BU13"/>
-    <mergeCell ref="BM14:BM15"/>
-    <mergeCell ref="BN14:BN15"/>
-    <mergeCell ref="BO14:BO15"/>
-    <mergeCell ref="BP14:BP15"/>
-    <mergeCell ref="BQ14:BU14"/>
-    <mergeCell ref="BD13:BL13"/>
-    <mergeCell ref="BD14:BD15"/>
-    <mergeCell ref="BE14:BE15"/>
-    <mergeCell ref="BF14:BF15"/>
-    <mergeCell ref="BG14:BG15"/>
-    <mergeCell ref="BH14:BL14"/>
-    <mergeCell ref="AL13:AT13"/>
-    <mergeCell ref="AL14:AL15"/>
-    <mergeCell ref="AM14:AM15"/>
-    <mergeCell ref="AN14:AN15"/>
-    <mergeCell ref="AO14:AO15"/>
-    <mergeCell ref="AP14:AT14"/>
-    <mergeCell ref="AY14:BC14"/>
+  <mergeCells count="73">
+    <mergeCell ref="B13:B15"/>
+    <mergeCell ref="A13:A15"/>
+    <mergeCell ref="N14:R14"/>
+    <mergeCell ref="CU13:CU15"/>
+    <mergeCell ref="S13:Z13"/>
+    <mergeCell ref="V14:Z14"/>
+    <mergeCell ref="AA13:AI13"/>
+    <mergeCell ref="AA14:AA15"/>
+    <mergeCell ref="AB14:AB15"/>
+    <mergeCell ref="AE14:AI14"/>
+    <mergeCell ref="U14:U15"/>
+    <mergeCell ref="T14:T15"/>
+    <mergeCell ref="C13:C15"/>
+    <mergeCell ref="J13:J15"/>
+    <mergeCell ref="D13:F13"/>
+    <mergeCell ref="G13:I13"/>
+    <mergeCell ref="CV13:CV15"/>
+    <mergeCell ref="CW13:CW15"/>
+    <mergeCell ref="AC14:AC15"/>
+    <mergeCell ref="AD14:AD15"/>
+    <mergeCell ref="K13:R13"/>
+    <mergeCell ref="K14:K15"/>
+    <mergeCell ref="L14:L15"/>
+    <mergeCell ref="M14:M15"/>
+    <mergeCell ref="S14:S15"/>
+    <mergeCell ref="AS13:BA13"/>
+    <mergeCell ref="AS14:AS15"/>
+    <mergeCell ref="AT14:AT15"/>
+    <mergeCell ref="AU14:AU15"/>
+    <mergeCell ref="AV14:AV15"/>
+    <mergeCell ref="AW14:BA14"/>
     <mergeCell ref="D14:D15"/>
     <mergeCell ref="E14:E15"/>
     <mergeCell ref="F14:F15"/>
     <mergeCell ref="G14:G15"/>
     <mergeCell ref="H14:H15"/>
     <mergeCell ref="I14:I15"/>
-    <mergeCell ref="G13:I13"/>
-    <mergeCell ref="CX13:CX15"/>
-    <mergeCell ref="CY13:CY15"/>
-    <mergeCell ref="AE14:AE15"/>
-    <mergeCell ref="AF14:AF15"/>
-    <mergeCell ref="K13:S13"/>
-    <mergeCell ref="K14:K15"/>
-    <mergeCell ref="L14:L15"/>
-    <mergeCell ref="M14:M15"/>
-    <mergeCell ref="N14:N15"/>
-    <mergeCell ref="T14:T15"/>
-    <mergeCell ref="AU13:BC13"/>
-    <mergeCell ref="AU14:AU15"/>
-    <mergeCell ref="AV14:AV15"/>
-    <mergeCell ref="AW14:AW15"/>
-    <mergeCell ref="AX14:AX15"/>
-    <mergeCell ref="B13:B15"/>
-    <mergeCell ref="A13:A15"/>
-    <mergeCell ref="O14:S14"/>
-    <mergeCell ref="CW13:CW15"/>
-    <mergeCell ref="T13:AB13"/>
-    <mergeCell ref="X14:AB14"/>
-    <mergeCell ref="AC13:AK13"/>
-    <mergeCell ref="AC14:AC15"/>
-    <mergeCell ref="AD14:AD15"/>
-    <mergeCell ref="AG14:AK14"/>
-    <mergeCell ref="W14:W15"/>
-    <mergeCell ref="V14:V15"/>
-    <mergeCell ref="U14:U15"/>
-    <mergeCell ref="C13:C15"/>
-    <mergeCell ref="J13:J15"/>
-    <mergeCell ref="D13:F13"/>
+    <mergeCell ref="AJ13:AR13"/>
+    <mergeCell ref="AJ14:AJ15"/>
+    <mergeCell ref="AK14:AK15"/>
+    <mergeCell ref="AL14:AL15"/>
+    <mergeCell ref="AM14:AM15"/>
+    <mergeCell ref="AN14:AR14"/>
+    <mergeCell ref="BB13:BJ13"/>
+    <mergeCell ref="BB14:BB15"/>
+    <mergeCell ref="BC14:BC15"/>
+    <mergeCell ref="BD14:BD15"/>
+    <mergeCell ref="BE14:BE15"/>
+    <mergeCell ref="BF14:BJ14"/>
+    <mergeCell ref="BK13:BS13"/>
+    <mergeCell ref="BK14:BK15"/>
+    <mergeCell ref="BL14:BL15"/>
+    <mergeCell ref="BM14:BM15"/>
+    <mergeCell ref="BN14:BN15"/>
+    <mergeCell ref="BO14:BS14"/>
+    <mergeCell ref="BT13:CB13"/>
+    <mergeCell ref="BT14:BT15"/>
+    <mergeCell ref="BU14:BU15"/>
+    <mergeCell ref="BV14:BV15"/>
+    <mergeCell ref="BW14:BW15"/>
+    <mergeCell ref="BX14:CB14"/>
+    <mergeCell ref="CC13:CK13"/>
+    <mergeCell ref="CC14:CC15"/>
+    <mergeCell ref="CD14:CD15"/>
+    <mergeCell ref="CE14:CE15"/>
+    <mergeCell ref="CF14:CF15"/>
+    <mergeCell ref="CG14:CK14"/>
+    <mergeCell ref="CL13:CT13"/>
+    <mergeCell ref="CL14:CL15"/>
+    <mergeCell ref="CM14:CM15"/>
+    <mergeCell ref="CN14:CN15"/>
+    <mergeCell ref="CO14:CO15"/>
+    <mergeCell ref="CP14:CT14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId1"/>

</xml_diff>